<commit_message>
Implemented conditional (issue #4). Reworked time handling. Fixed exponent handling. Fixed formatting.xlsx.
</commit_message>
<xml_diff>
--- a/backend/test/assets/formatting.xlsx
+++ b/backend/test/assets/formatting.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23507"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_50FC12B005E796F1B2322BBBB1879748210656A3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
     <sheet name="datetime" sheetId="3" r:id="rId3"/>
     <sheet name="fraction" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,6 +43,51 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Formatted</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0.00;[Red]0.00</t>
+  </si>
+  <si>
+    <t>0.00_);(0.00)</t>
+  </si>
+  <si>
+    <t>0.00_);[Red](0.00)</t>
+  </si>
+  <si>
+    <t>"$"#,##0.00</t>
+  </si>
+  <si>
+    <t>"$"#,##0.00;[Red]"$"#,##0.00</t>
+  </si>
+  <si>
+    <t>"$"#,##0.00_);("$"#,##0.00)</t>
+  </si>
+  <si>
+    <t>"$"#,##0.00_);[Red]("$"#,##0.00)</t>
+  </si>
+  <si>
+    <t>#,##0.00 [$€-40C]</t>
+  </si>
+  <si>
+    <t>[$PLN] #,##0.00</t>
+  </si>
+  <si>
+    <t>[$₹-439]#,##0.00</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>#,##0%</t>
+  </si>
+  <si>
     <t>0.00E+00</t>
   </si>
   <si>
@@ -54,7 +100,22 @@
     <t>##0.0E+0</t>
   </si>
   <si>
+    <t># ?/2</t>
+  </si>
+  <si>
     <t>000.000.000.000</t>
+  </si>
+  <si>
+    <t>[&lt;=9999999]###-##-##;(###) ###-##-##</t>
+  </si>
+  <si>
+    <t>[&lt;=999999]###-###;(###) ###-###</t>
+  </si>
+  <si>
+    <t>00000000000</t>
+  </si>
+  <si>
+    <t>000-000-00-00</t>
   </si>
   <si>
     <t>mm-dd-yy</t>
@@ -135,76 +196,7 @@
     <t>[$-40C]dd-mmm-yy;@</t>
   </si>
   <si>
-    <t>Formatted</t>
-  </si>
-  <si>
     <t>[$-415]mmmmm.yy;@</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>0.00;[Red]0.00</t>
-  </si>
-  <si>
-    <t>0.00_);(0.00)</t>
-  </si>
-  <si>
-    <t>0.00_);[Red](0.00)</t>
-  </si>
-  <si>
-    <t>$#,##0.00</t>
-  </si>
-  <si>
-    <t>$#,##0.00;[Red]$#,##0.00</t>
-  </si>
-  <si>
-    <t>$#,##0.00_);($#,##0.00)</t>
-  </si>
-  <si>
-    <t>$#,##0.00_);[Red]($#,##0.00)</t>
-  </si>
-  <si>
-    <t>#,##0.00 [$€-40C]</t>
-  </si>
-  <si>
-    <t>[$PLN] #,##0.00</t>
-  </si>
-  <si>
-    <t>[$₹-439]#,##0.00</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>#,##0%</t>
-  </si>
-  <si>
-    <t># ?/2</t>
-  </si>
-  <si>
-    <t>[&lt;=9999999]###-##-##;(###) ###-##-##</t>
-  </si>
-  <si>
-    <t>[&lt;=999999]###-###;(###) ###-###</t>
-  </si>
-  <si>
-    <t>00000000000</t>
-  </si>
-  <si>
-    <t>000-000-00-00</t>
-  </si>
-  <si>
-    <t># ???/???</t>
-  </si>
-  <si>
-    <t># ??/??</t>
-  </si>
-  <si>
-    <t># ?/?</t>
   </si>
   <si>
     <t>[h]</t>
@@ -218,11 +210,20 @@
   <si>
     <t>mm</t>
   </si>
+  <si>
+    <t># ???/???</t>
+  </si>
+  <si>
+    <t># ??/??</t>
+  </si>
+  <si>
+    <t># ?/?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="51">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -271,10 +272,10 @@
     <numFmt numFmtId="206" formatCode="00000000000"/>
     <numFmt numFmtId="207" formatCode="000\-000\-00\-00"/>
     <numFmt numFmtId="208" formatCode="#\ ???/???"/>
-    <numFmt numFmtId="211" formatCode="[h]"/>
-    <numFmt numFmtId="213" formatCode="[mm]"/>
-    <numFmt numFmtId="214" formatCode="[sss]"/>
-    <numFmt numFmtId="215" formatCode="mm"/>
+    <numFmt numFmtId="209" formatCode="[h]"/>
+    <numFmt numFmtId="210" formatCode="[mm]"/>
+    <numFmt numFmtId="211" formatCode="[sss]"/>
+    <numFmt numFmtId="212" formatCode="mm"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -386,10 +387,10 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="209" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +451,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -502,7 +503,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -696,18 +697,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -728,12 +729,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>123.45</v>
@@ -749,7 +750,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>123.45</v>
@@ -765,7 +766,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>-123.45</v>
@@ -781,7 +782,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>-123.45</v>
@@ -797,7 +798,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>123.45</v>
@@ -813,7 +814,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>12345.67</v>
@@ -829,7 +830,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>12345.67</v>
@@ -845,7 +846,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>12345.67</v>
@@ -861,7 +862,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>12345.67</v>
@@ -877,7 +878,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>12345.67</v>
@@ -893,7 +894,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>12345.67</v>
@@ -909,7 +910,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>12345.67</v>
@@ -925,7 +926,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>0.34</v>
@@ -941,7 +942,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0.34</v>
@@ -957,7 +958,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>1234.3399999999999</v>
@@ -973,7 +974,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>1500000</v>
@@ -989,7 +990,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>4.35E-5</v>
@@ -1005,7 +1006,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>1500000</v>
@@ -1021,7 +1022,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>150000</v>
@@ -1037,7 +1038,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>150000</v>
@@ -1053,7 +1054,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>0.123</v>
@@ -1069,7 +1070,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>0.55000000000000004</v>
@@ -1085,7 +1086,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>1.123</v>
@@ -1097,36 +1098,6 @@
       <c r="D24" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">1    </v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="D25" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="D26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="D27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="D28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="D29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1166,12 +1137,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>1234567890.1229999</v>
@@ -1187,7 +1158,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>1234567</v>
@@ -1203,7 +1174,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>123456</v>
@@ -1219,7 +1190,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>123456789</v>
@@ -1235,7 +1206,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>123456789</v>
@@ -1251,7 +1222,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>123456789</v>
@@ -1276,11 +1247,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1303,12 +1274,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7">
         <v>40867</v>
@@ -1324,7 +1295,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>40868</v>
@@ -1334,13 +1305,13 @@
         <v>40868</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D34" si="1">TEXT(B3, A3)</f>
+        <f t="shared" ref="D3:D35" si="1">TEXT(B3, A3)</f>
         <v>Monday, November 21, 2011</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B4" s="7">
         <v>40869</v>
@@ -1356,7 +1327,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7">
         <v>40870</v>
@@ -1372,7 +1343,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B6" s="7">
         <v>40871</v>
@@ -1388,7 +1359,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7">
         <v>40872</v>
@@ -1404,7 +1375,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7">
         <v>40873</v>
@@ -1420,7 +1391,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B9" s="7">
         <v>40874</v>
@@ -1436,7 +1407,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B10" s="7">
         <v>40875</v>
@@ -1452,7 +1423,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7">
         <v>40876</v>
@@ -1468,7 +1439,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7">
         <v>40877</v>
@@ -1484,7 +1455,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B13" s="7">
         <v>40878</v>
@@ -1500,7 +1471,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7">
         <v>40879</v>
@@ -1516,7 +1487,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B15" s="7">
         <v>40880.271701388898</v>
@@ -1532,7 +1503,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7">
         <v>40881.271701388891</v>
@@ -1548,7 +1519,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B17" s="7">
         <v>40882.271701388891</v>
@@ -1564,7 +1535,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B18" s="7">
         <v>40883.271701388891</v>
@@ -1580,7 +1551,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B19" s="7">
         <v>40884.271701388891</v>
@@ -1596,7 +1567,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B20" s="7">
         <v>40885.271701388891</v>
@@ -1612,7 +1583,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B21" s="7">
         <v>40886.271701388891</v>
@@ -1628,7 +1599,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B22" s="7">
         <v>40887.271701388891</v>
@@ -1644,7 +1615,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B23" s="7">
         <v>40888.271701388891</v>
@@ -1660,7 +1631,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B24" s="7">
         <v>40889.271707175925</v>
@@ -1676,7 +1647,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B25" s="7">
         <v>40890.271701388891</v>
@@ -1692,7 +1663,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B26" s="7">
         <v>40891.271701388891</v>
@@ -1708,7 +1679,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B27" s="7">
         <v>40892.271701388891</v>
@@ -1724,7 +1695,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B28" s="7">
         <v>40893.271701388891</v>
@@ -1740,7 +1711,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B29" s="7">
         <v>40894.271701388891</v>
@@ -1756,7 +1727,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B30" s="7">
         <v>40895.271701388891</v>
@@ -1772,7 +1743,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31" s="7">
         <v>25569</v>
@@ -1788,7 +1759,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B32" s="7">
         <v>25569</v>
@@ -1804,7 +1775,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7">
         <v>25569</v>
@@ -1820,7 +1791,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" s="7">
         <v>40895.271701388891</v>
@@ -1845,7 +1816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D394"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1865,12 +1836,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -1886,7 +1857,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>2E-3</v>
@@ -1902,7 +1873,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>3.0000000000000001E-3</v>
@@ -1918,7 +1889,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>4.0000000000000001E-3</v>
@@ -1934,7 +1905,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>5.0000000000000001E-3</v>
@@ -1950,7 +1921,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>6.0000000000000001E-3</v>
@@ -1966,7 +1937,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>7.0000000000000001E-3</v>
@@ -1982,7 +1953,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>8.0000000000000002E-3</v>
@@ -1998,7 +1969,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>8.9999999999999993E-3</v>
@@ -2014,7 +1985,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>0.01</v>
@@ -2030,7 +2001,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>1.0999999999999999E-2</v>
@@ -2046,7 +2017,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>1.2E-2</v>
@@ -2062,7 +2033,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>1.2999999999999999E-2</v>
@@ -2078,7 +2049,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>1.4E-2</v>
@@ -2094,7 +2065,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>1.4999999999999999E-2</v>
@@ -2110,7 +2081,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>1.6E-2</v>
@@ -2126,7 +2097,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>1.7000000000000001E-2</v>
@@ -2142,7 +2113,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>1.7999999999999999E-2</v>
@@ -2158,7 +2129,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B20">
         <v>1.9E-2</v>
@@ -2174,7 +2145,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B21">
         <v>0.02</v>
@@ -2190,7 +2161,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B22">
         <v>2.1000000000000001E-2</v>
@@ -2206,7 +2177,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>2.1999999999999999E-2</v>
@@ -2222,7 +2193,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B24">
         <v>2.3E-2</v>
@@ -2238,7 +2209,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>2.4E-2</v>
@@ -2254,7 +2225,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
@@ -2270,7 +2241,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>2.5999999999999999E-2</v>
@@ -2286,7 +2257,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B28">
         <v>2.7E-2</v>
@@ -2302,7 +2273,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B29">
         <v>2.8000000000000001E-2</v>
@@ -2318,7 +2289,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B30">
         <v>2.9000000000000001E-2</v>
@@ -2334,7 +2305,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>0.03</v>
@@ -2350,7 +2321,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B32">
         <v>3.1E-2</v>
@@ -2366,7 +2337,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B33">
         <v>3.2000000000000001E-2</v>
@@ -2382,7 +2353,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>3.3000000000000002E-2</v>
@@ -2398,7 +2369,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B35">
         <v>3.4000000000000002E-2</v>
@@ -2414,7 +2385,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <v>3.5000000000000003E-2</v>
@@ -2430,7 +2401,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>3.5999999999999997E-2</v>
@@ -2446,7 +2417,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B38">
         <v>3.6999999999999998E-2</v>
@@ -2462,7 +2433,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B39">
         <v>3.7999999999999999E-2</v>
@@ -2478,7 +2449,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B40">
         <v>3.9E-2</v>
@@ -2494,7 +2465,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B41">
         <v>0.04</v>
@@ -2510,7 +2481,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B42">
         <v>4.1000000000000002E-2</v>
@@ -2526,7 +2497,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>4.2000000000000003E-2</v>
@@ -2542,7 +2513,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B44">
         <v>4.2999999999999997E-2</v>
@@ -2558,7 +2529,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B45">
         <v>4.3999999999999997E-2</v>
@@ -2574,7 +2545,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B46">
         <v>4.4999999999999998E-2</v>
@@ -2590,7 +2561,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B47">
         <v>4.5999999999999999E-2</v>
@@ -2606,7 +2577,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B48">
         <v>4.7E-2</v>
@@ -2622,7 +2593,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>4.8000000000000001E-2</v>
@@ -2638,7 +2609,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B50">
         <v>4.9000000000000002E-2</v>
@@ -2654,7 +2625,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B51">
         <v>0.05</v>
@@ -2670,7 +2641,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B52">
         <v>5.0999999999999997E-2</v>
@@ -2686,7 +2657,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B53">
         <v>5.1999999999999998E-2</v>
@@ -2702,7 +2673,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>5.2999999999999999E-2</v>
@@ -2718,7 +2689,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>5.3999999999999999E-2</v>
@@ -2734,7 +2705,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>5.5E-2</v>
@@ -2750,7 +2721,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>5.6000000000000001E-2</v>
@@ -2766,7 +2737,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>5.7000000000000002E-2</v>
@@ -2782,7 +2753,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>5.8000000000000003E-2</v>
@@ -2798,7 +2769,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B60">
         <v>5.8999999999999997E-2</v>
@@ -2814,7 +2785,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>0.06</v>
@@ -2830,7 +2801,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>6.0999999999999999E-2</v>
@@ -2846,7 +2817,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B63">
         <v>6.2E-2</v>
@@ -2862,7 +2833,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B64">
         <v>6.3E-2</v>
@@ -2878,7 +2849,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B65">
         <v>6.4000000000000001E-2</v>
@@ -2894,7 +2865,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B66">
         <v>6.5000000000000002E-2</v>
@@ -2910,7 +2881,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B67">
         <v>6.6000000000000003E-2</v>
@@ -2926,7 +2897,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B68">
         <v>6.7000000000000004E-2</v>
@@ -2942,7 +2913,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B69">
         <v>6.8000000000000005E-2</v>
@@ -2958,7 +2929,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B70">
         <v>6.9000000000000006E-2</v>
@@ -2974,7 +2945,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B71">
         <v>7.0000000000000007E-2</v>
@@ -2990,7 +2961,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B72">
         <v>7.0999999999999994E-2</v>
@@ -3006,7 +2977,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B73">
         <v>7.1999999999999995E-2</v>
@@ -3022,7 +2993,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B74">
         <v>7.2999999999999995E-2</v>
@@ -3038,7 +3009,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B75">
         <v>7.3999999999999996E-2</v>
@@ -3054,7 +3025,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B76">
         <v>7.4999999999999997E-2</v>
@@ -3070,7 +3041,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B77">
         <v>7.5999999999999998E-2</v>
@@ -3086,7 +3057,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B78">
         <v>7.6999999999999999E-2</v>
@@ -3102,7 +3073,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B79">
         <v>7.8E-2</v>
@@ -3118,7 +3089,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B80">
         <v>7.9000000000000001E-2</v>
@@ -3134,7 +3105,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B81">
         <v>0.08</v>
@@ -3150,7 +3121,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B82">
         <v>8.1000000000000003E-2</v>
@@ -3166,7 +3137,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B83">
         <v>8.2000000000000003E-2</v>
@@ -3182,7 +3153,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B84">
         <v>8.3000000000000004E-2</v>
@@ -3198,7 +3169,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B85">
         <v>8.4000000000000005E-2</v>
@@ -3214,7 +3185,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B86">
         <v>8.5000000000000006E-2</v>
@@ -3230,7 +3201,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B87">
         <v>8.5999999999999993E-2</v>
@@ -3246,7 +3217,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B88">
         <v>8.6999999999999994E-2</v>
@@ -3262,7 +3233,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B89">
         <v>8.7999999999999995E-2</v>
@@ -3278,7 +3249,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B90">
         <v>8.8999999999999996E-2</v>
@@ -3294,7 +3265,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B91">
         <v>0.09</v>
@@ -3310,7 +3281,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B92">
         <v>9.0999999999999998E-2</v>
@@ -3326,7 +3297,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B93">
         <v>9.1999999999999998E-2</v>
@@ -3342,7 +3313,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B94">
         <v>9.2999999999999999E-2</v>
@@ -3358,7 +3329,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B95">
         <v>9.4E-2</v>
@@ -3374,7 +3345,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B96">
         <v>9.5000000000000001E-2</v>
@@ -3390,7 +3361,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B97">
         <v>9.6000000000000002E-2</v>
@@ -3406,7 +3377,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B98">
         <v>9.7000000000000003E-2</v>
@@ -3422,7 +3393,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B99">
         <v>9.8000000000000004E-2</v>
@@ -3438,7 +3409,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B100">
         <v>9.9000000000000005E-2</v>
@@ -3454,7 +3425,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B101">
         <v>0.62</v>
@@ -3470,7 +3441,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B102">
         <v>0.621</v>
@@ -3486,7 +3457,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B103">
         <v>0.622</v>
@@ -3502,7 +3473,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B104">
         <v>0.623</v>
@@ -3518,7 +3489,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B105">
         <v>0.624</v>
@@ -3534,7 +3505,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B106">
         <v>0.625</v>
@@ -3550,7 +3521,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B107">
         <v>0.626</v>
@@ -3566,7 +3537,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B108">
         <v>0.627</v>
@@ -3582,7 +3553,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B109">
         <v>0.628</v>
@@ -3598,7 +3569,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B110">
         <v>0.629</v>
@@ -3614,7 +3585,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B111">
         <v>0.63</v>
@@ -3630,7 +3601,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B112">
         <v>0.63100000000000001</v>
@@ -3646,7 +3617,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B113">
         <v>0.63200000000000001</v>
@@ -3662,7 +3633,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B114">
         <v>0.63300000000000001</v>
@@ -3678,7 +3649,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B115">
         <v>0.63400000000000001</v>
@@ -3694,7 +3665,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B116">
         <v>0.63500000000000001</v>
@@ -3710,7 +3681,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B117">
         <v>0.63600000000000001</v>
@@ -3726,7 +3697,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B118">
         <v>0.63700000000000001</v>
@@ -3742,7 +3713,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B119">
         <v>0.63800000000000001</v>
@@ -3758,7 +3729,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B120">
         <v>0.63900000000000001</v>
@@ -3774,7 +3745,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B121">
         <v>0.64</v>
@@ -3790,7 +3761,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B122">
         <v>0.64100000000000001</v>
@@ -3806,7 +3777,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B123">
         <v>0.64200000000000002</v>
@@ -3822,7 +3793,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B124">
         <v>0.64300000000000002</v>
@@ -3838,7 +3809,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B125">
         <v>0.64400000000000002</v>
@@ -3854,7 +3825,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B126">
         <v>0.64500000000000002</v>
@@ -3870,7 +3841,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B127">
         <v>0.64600000000000002</v>
@@ -3886,7 +3857,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B128">
         <v>0.64700000000000002</v>
@@ -3902,7 +3873,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B129">
         <v>0.64800000000000002</v>
@@ -3918,7 +3889,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B130">
         <v>0.64900000000000002</v>
@@ -3934,7 +3905,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B131">
         <v>0.65</v>
@@ -3950,7 +3921,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B132">
         <v>0.65100000000000002</v>
@@ -3966,7 +3937,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B133">
         <v>0.65200000000000002</v>
@@ -3982,7 +3953,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B134">
         <v>0.65300000000000002</v>
@@ -3998,7 +3969,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B135">
         <v>0.65400000000000003</v>
@@ -4014,7 +3985,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B136">
         <v>0.65500000000000003</v>
@@ -4030,7 +4001,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B137">
         <v>0.65600000000000003</v>
@@ -4046,7 +4017,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B138">
         <v>0.65700000000000003</v>
@@ -4062,7 +4033,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B139">
         <v>0.65800000000000003</v>
@@ -4078,7 +4049,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B140">
         <v>0.65900000000000003</v>
@@ -4094,7 +4065,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B141">
         <v>0.66</v>
@@ -4110,7 +4081,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B142">
         <v>0.66100000000000003</v>
@@ -4126,7 +4097,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B143">
         <v>0.66200000000000003</v>
@@ -4142,7 +4113,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B144">
         <v>0.66300000000000003</v>
@@ -4158,7 +4129,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B145">
         <v>0.66400000000000003</v>
@@ -4174,7 +4145,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B146">
         <v>0.66500000000000004</v>
@@ -4190,7 +4161,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B147">
         <v>0.66600000000000004</v>
@@ -4206,7 +4177,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B148">
         <v>0.66700000000000004</v>
@@ -4222,7 +4193,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B149">
         <v>0.66800000000000004</v>
@@ -4238,7 +4209,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B150">
         <v>0.66900000000000004</v>
@@ -4254,7 +4225,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B151">
         <v>0.67</v>
@@ -4270,7 +4241,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B152">
         <v>0.67100000000000004</v>
@@ -4286,7 +4257,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B153">
         <v>0.67200000000000004</v>
@@ -4302,7 +4273,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B154">
         <v>0.67300000000000004</v>
@@ -4318,7 +4289,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B155">
         <v>0.67400000000000004</v>
@@ -4334,7 +4305,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B156">
         <v>0.67500000000000004</v>
@@ -4350,7 +4321,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B157">
         <v>0.67600000000000005</v>
@@ -4366,7 +4337,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B158">
         <v>0.67700000000000005</v>
@@ -4382,7 +4353,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B159">
         <v>0.67800000000000005</v>
@@ -4398,7 +4369,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B160">
         <v>0.67900000000000005</v>
@@ -4414,7 +4385,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B161">
         <v>0.68</v>
@@ -4430,7 +4401,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B162">
         <v>0.68100000000000005</v>
@@ -4446,7 +4417,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B163">
         <v>0.68200000000000005</v>
@@ -4462,7 +4433,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B164">
         <v>0.68300000000000005</v>
@@ -4478,7 +4449,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B165">
         <v>0.68400000000000005</v>
@@ -4494,7 +4465,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B166">
         <v>0.68500000000000005</v>
@@ -4510,7 +4481,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B167">
         <v>0.68600000000000005</v>
@@ -4526,7 +4497,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B168">
         <v>0.68700000000000006</v>
@@ -4542,7 +4513,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B169">
         <v>0.68799999999999994</v>
@@ -4558,7 +4529,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B170">
         <v>0.68899999999999995</v>
@@ -4574,7 +4545,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B171">
         <v>0.69</v>
@@ -4590,7 +4561,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B172">
         <v>0.69099999999999995</v>
@@ -4606,7 +4577,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B173">
         <v>0.69199999999999995</v>
@@ -4622,7 +4593,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B174">
         <v>0.69299999999999995</v>
@@ -4638,7 +4609,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B175">
         <v>0.69399999999999995</v>
@@ -4654,7 +4625,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B176">
         <v>0.69499999999999995</v>
@@ -4670,7 +4641,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B177">
         <v>0.69599999999999995</v>
@@ -4686,7 +4657,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B178">
         <v>0.69699999999999995</v>
@@ -4702,7 +4673,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B179">
         <v>0.69799999999999995</v>
@@ -4718,7 +4689,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B180">
         <v>0.69899999999999995</v>
@@ -4734,7 +4705,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B181">
         <v>0.7</v>
@@ -4750,7 +4721,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B182">
         <v>0.70099999999999996</v>
@@ -4766,7 +4737,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B183">
         <v>0.70199999999999996</v>
@@ -4782,7 +4753,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B184">
         <v>0.70299999999999996</v>
@@ -4798,7 +4769,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B185">
         <v>0.70399999999999996</v>
@@ -4814,7 +4785,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B186">
         <v>0.70499999999999996</v>
@@ -4830,7 +4801,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B187">
         <v>0.70599999999999996</v>
@@ -4846,7 +4817,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B188">
         <v>0.70699999999999996</v>
@@ -4862,7 +4833,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B189">
         <v>0.70799999999999996</v>
@@ -4878,7 +4849,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B190">
         <v>0.70899999999999996</v>
@@ -4894,7 +4865,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B191">
         <v>0.71</v>
@@ -4910,7 +4881,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B192">
         <v>0.71099999999999997</v>
@@ -4926,7 +4897,7 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B193">
         <v>0.71199999999999997</v>
@@ -4942,7 +4913,7 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B194">
         <v>0.71299999999999997</v>
@@ -4958,7 +4929,7 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B195">
         <v>0.71399999999999997</v>
@@ -4974,7 +4945,7 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B196">
         <v>0.71499999999999997</v>
@@ -4990,7 +4961,7 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B197">
         <v>0.71599999999999997</v>
@@ -5006,7 +4977,7 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B198">
         <v>0.71699999999999997</v>
@@ -5022,7 +4993,7 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B199">
         <v>0.71799999999999997</v>
@@ -5038,7 +5009,7 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B200">
         <v>0.71899999999999997</v>
@@ -5054,7 +5025,7 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B201">
         <v>0.99</v>
@@ -5070,7 +5041,7 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B202">
         <v>0.99099999999999999</v>
@@ -5086,7 +5057,7 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B203">
         <v>0.99199999999999999</v>
@@ -5102,7 +5073,7 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B204">
         <v>0.99299999999999999</v>
@@ -5118,7 +5089,7 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B205">
         <v>0.99399999999999999</v>
@@ -5134,7 +5105,7 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B206">
         <v>0.995</v>
@@ -5150,7 +5121,7 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B207">
         <v>0.996</v>
@@ -5166,7 +5137,7 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B208">
         <v>0.997</v>
@@ -5182,7 +5153,7 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B209">
         <v>0.998</v>
@@ -5198,7 +5169,7 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B210">
         <v>0.999</v>
@@ -5214,7 +5185,7 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -5230,7 +5201,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B212">
         <v>9.5000000000000001E-2</v>
@@ -5246,7 +5217,7 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B213">
         <v>9.6000000000000002E-2</v>
@@ -5262,7 +5233,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B214">
         <v>9.7000000000000003E-2</v>
@@ -5278,7 +5249,7 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B215">
         <v>9.8000000000000004E-2</v>
@@ -5294,7 +5265,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B216">
         <v>9.9000000000000005E-2</v>
@@ -5310,7 +5281,7 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B217">
         <v>0.1</v>
@@ -5326,7 +5297,7 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B218">
         <v>0.10100000000000001</v>
@@ -5342,7 +5313,7 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B219">
         <v>0.10199999999999999</v>
@@ -5358,7 +5329,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B220">
         <v>0.10299999999999999</v>
@@ -5374,7 +5345,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B221">
         <v>0.104</v>
@@ -5390,7 +5361,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B222">
         <v>0.105</v>
@@ -5406,7 +5377,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B223">
         <v>0.106</v>
@@ -5422,7 +5393,7 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B224">
         <v>0.107</v>
@@ -5438,7 +5409,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B225">
         <v>0.108</v>
@@ -5454,7 +5425,7 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B226">
         <v>0.109</v>
@@ -5470,7 +5441,7 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B227">
         <v>0.11</v>
@@ -5486,7 +5457,7 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B228">
         <v>0.111</v>
@@ -5502,7 +5473,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B229">
         <v>0.112</v>
@@ -5518,7 +5489,7 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B230">
         <v>0.113</v>
@@ -5534,7 +5505,7 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B231">
         <v>0.114</v>
@@ -5550,7 +5521,7 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B232">
         <v>0.115</v>
@@ -5566,7 +5537,7 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B233">
         <v>0.11600000000000001</v>
@@ -5582,7 +5553,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B234">
         <v>0.11700000000000001</v>
@@ -5598,7 +5569,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B235">
         <v>0.11799999999999999</v>
@@ -5614,7 +5585,7 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B236">
         <v>0.11899999999999999</v>
@@ -5630,7 +5601,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B237">
         <v>0.12</v>
@@ -5646,7 +5617,7 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B238">
         <v>0.121</v>
@@ -5662,7 +5633,7 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B239">
         <v>0.122</v>
@@ -5678,7 +5649,7 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B240">
         <v>0.123</v>
@@ -5694,7 +5665,7 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B241">
         <v>0.124</v>
@@ -5710,7 +5681,7 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B242">
         <v>0.49</v>
@@ -5726,7 +5697,7 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B243">
         <v>0.49099999999999999</v>
@@ -5742,7 +5713,7 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B244">
         <v>0.49199999999999999</v>
@@ -5758,7 +5729,7 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B245">
         <v>0.49299999999999999</v>
@@ -5774,7 +5745,7 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B246">
         <v>0.49399999999999999</v>
@@ -5790,7 +5761,7 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B247">
         <v>0.495</v>
@@ -5806,7 +5777,7 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B248">
         <v>0.496</v>
@@ -5822,7 +5793,7 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B249">
         <v>0.497</v>
@@ -5838,7 +5809,7 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B250">
         <v>0.498</v>
@@ -5854,7 +5825,7 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B251">
         <v>0.499</v>
@@ -5870,7 +5841,7 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B252">
         <v>0.5</v>
@@ -5886,7 +5857,7 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B253">
         <v>0.501</v>
@@ -5902,7 +5873,7 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B254">
         <v>0.502</v>
@@ -5918,7 +5889,7 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B255">
         <v>0.503</v>
@@ -5934,7 +5905,7 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B256">
         <v>0.504</v>
@@ -5950,7 +5921,7 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B257">
         <v>0.505</v>
@@ -5966,7 +5937,7 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B258">
         <v>0.50600000000000001</v>
@@ -5982,7 +5953,7 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B259">
         <v>0.50700000000000001</v>
@@ -5998,7 +5969,7 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B260">
         <v>0.50800000000000001</v>
@@ -6014,7 +5985,7 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B261">
         <v>0.50900000000000001</v>
@@ -6030,7 +6001,7 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B262">
         <v>0.51</v>
@@ -6046,7 +6017,7 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B263">
         <v>0.51100000000000001</v>
@@ -6062,7 +6033,7 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B264">
         <v>0.51200000000000001</v>
@@ -6078,7 +6049,7 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B265">
         <v>0.51300000000000001</v>
@@ -6094,7 +6065,7 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B266">
         <v>0.51400000000000001</v>
@@ -6110,7 +6081,7 @@
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B267">
         <v>0.51500000000000001</v>
@@ -6126,7 +6097,7 @@
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B268">
         <v>0.51600000000000001</v>
@@ -6142,7 +6113,7 @@
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B269">
         <v>0.51700000000000002</v>
@@ -6158,7 +6129,7 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B270">
         <v>0.51800000000000002</v>
@@ -6174,7 +6145,7 @@
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B271">
         <v>0.51900000000000002</v>
@@ -6190,7 +6161,7 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B272">
         <v>0.52</v>
@@ -6206,7 +6177,7 @@
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B273">
         <v>0.97499999999999998</v>
@@ -6222,7 +6193,7 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B274">
         <v>0.97599999999999998</v>
@@ -6238,7 +6209,7 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B275">
         <v>0.97699999999999998</v>
@@ -6254,7 +6225,7 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B276">
         <v>0.97799999999999998</v>
@@ -6270,7 +6241,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B277">
         <v>0.97899999999999998</v>
@@ -6286,7 +6257,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B278">
         <v>0.98</v>
@@ -6302,7 +6273,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B279">
         <v>0.98099999999999998</v>
@@ -6318,7 +6289,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B280">
         <v>0.98199999999999998</v>
@@ -6334,7 +6305,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B281">
         <v>0.98299999999999998</v>
@@ -6350,7 +6321,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B282">
         <v>0.98399999999999999</v>
@@ -6366,7 +6337,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B283">
         <v>0.98499999999999999</v>
@@ -6382,7 +6353,7 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B284">
         <v>0.98599999999999999</v>
@@ -6398,7 +6369,7 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B285">
         <v>0.98699999999999999</v>
@@ -6414,7 +6385,7 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B286">
         <v>0.98799999999999999</v>
@@ -6430,7 +6401,7 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B287">
         <v>0.98899999999999999</v>
@@ -6446,7 +6417,7 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B288">
         <v>0.99</v>
@@ -6462,7 +6433,7 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B289">
         <v>0.99099999999999999</v>
@@ -6478,7 +6449,7 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B290">
         <v>0.99199999999999999</v>
@@ -6494,7 +6465,7 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B291">
         <v>0.99299999999999999</v>
@@ -6510,7 +6481,7 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B292">
         <v>0.99399999999999999</v>
@@ -6526,7 +6497,7 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B293">
         <v>9.8000000000000004E-2</v>
@@ -6542,7 +6513,7 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B294">
         <v>9.9000000000000005E-2</v>
@@ -6558,7 +6529,7 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B295">
         <v>0.1</v>
@@ -6574,7 +6545,7 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B296">
         <v>0.10100000000000001</v>
@@ -6590,7 +6561,7 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B297">
         <v>0.10199999999999999</v>
@@ -6606,7 +6577,7 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B298">
         <v>0.10299999999999999</v>
@@ -6622,7 +6593,7 @@
     </row>
     <row r="299" spans="1:4">
       <c r="A299" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B299">
         <v>0.115</v>
@@ -6638,7 +6609,7 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B300">
         <v>0.11600000000000001</v>
@@ -6654,7 +6625,7 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B301">
         <v>0.11700000000000001</v>
@@ -6670,7 +6641,7 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B302">
         <v>0.11799999999999999</v>
@@ -6686,7 +6657,7 @@
     </row>
     <row r="303" spans="1:4">
       <c r="A303" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B303">
         <v>0.11899999999999999</v>
@@ -6702,7 +6673,7 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B304">
         <v>0.12</v>
@@ -6718,7 +6689,7 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B305">
         <v>0.13100000000000001</v>
@@ -6734,7 +6705,7 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B306">
         <v>0.13200000000000001</v>
@@ -6750,7 +6721,7 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B307">
         <v>0.13300000000000001</v>
@@ -6766,7 +6737,7 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B308">
         <v>0.13400000000000001</v>
@@ -6782,7 +6753,7 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B309">
         <v>0.13500000000000001</v>
@@ -6798,7 +6769,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B310">
         <v>0.13600000000000001</v>
@@ -6814,7 +6785,7 @@
     </row>
     <row r="311" spans="1:4">
       <c r="A311" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B311">
         <v>0.151</v>
@@ -6830,7 +6801,7 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B312">
         <v>0.152</v>
@@ -6846,7 +6817,7 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B313">
         <v>0.153</v>
@@ -6862,7 +6833,7 @@
     </row>
     <row r="314" spans="1:4">
       <c r="A314" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B314">
         <v>0.154</v>
@@ -6878,7 +6849,7 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B315">
         <v>0.155</v>
@@ -6894,7 +6865,7 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B316">
         <v>0.156</v>
@@ -6910,7 +6881,7 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B317">
         <v>0.17899999999999999</v>
@@ -6926,7 +6897,7 @@
     </row>
     <row r="318" spans="1:4">
       <c r="A318" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B318">
         <v>0.18</v>
@@ -6942,7 +6913,7 @@
     </row>
     <row r="319" spans="1:4">
       <c r="A319" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B319">
         <v>0.18099999999999999</v>
@@ -6958,7 +6929,7 @@
     </row>
     <row r="320" spans="1:4">
       <c r="A320" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B320">
         <v>0.182</v>
@@ -6974,7 +6945,7 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B321">
         <v>0.183</v>
@@ -6990,7 +6961,7 @@
     </row>
     <row r="322" spans="1:4">
       <c r="A322" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B322">
         <v>0.184</v>
@@ -7006,7 +6977,7 @@
     </row>
     <row r="323" spans="1:4">
       <c r="A323" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B323">
         <v>0.21199999999999999</v>
@@ -7022,7 +6993,7 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B324">
         <v>0.21299999999999999</v>
@@ -7038,7 +7009,7 @@
     </row>
     <row r="325" spans="1:4">
       <c r="A325" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B325">
         <v>0.214</v>
@@ -7054,7 +7025,7 @@
     </row>
     <row r="326" spans="1:4">
       <c r="A326" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B326">
         <v>0.215</v>
@@ -7070,7 +7041,7 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B327">
         <v>0.216</v>
@@ -7086,7 +7057,7 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B328">
         <v>0.217</v>
@@ -7102,7 +7073,7 @@
     </row>
     <row r="329" spans="1:4">
       <c r="A329" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B329">
         <v>0.22800000000000001</v>
@@ -7118,7 +7089,7 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B330">
         <v>0.22900000000000001</v>
@@ -7134,7 +7105,7 @@
     </row>
     <row r="331" spans="1:4">
       <c r="A331" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B331">
         <v>0.23</v>
@@ -7150,7 +7121,7 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B332">
         <v>0.23100000000000001</v>
@@ -7166,7 +7137,7 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B333">
         <v>0.23200000000000001</v>
@@ -7182,7 +7153,7 @@
     </row>
     <row r="334" spans="1:4">
       <c r="A334" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B334">
         <v>0.23300000000000001</v>
@@ -7198,7 +7169,7 @@
     </row>
     <row r="335" spans="1:4">
       <c r="A335" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B335">
         <v>0.27</v>
@@ -7214,7 +7185,7 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B336">
         <v>0.27100000000000002</v>
@@ -7230,7 +7201,7 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B337">
         <v>0.27200000000000002</v>
@@ -7246,7 +7217,7 @@
     </row>
     <row r="338" spans="1:4">
       <c r="A338" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B338">
         <v>0.27300000000000002</v>
@@ -7262,7 +7233,7 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B339">
         <v>0.27400000000000002</v>
@@ -7278,7 +7249,7 @@
     </row>
     <row r="340" spans="1:4">
       <c r="A340" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B340">
         <v>0.27500000000000002</v>
@@ -7294,7 +7265,7 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B341">
         <v>0.29799999999999999</v>
@@ -7310,7 +7281,7 @@
     </row>
     <row r="342" spans="1:4">
       <c r="A342" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B342">
         <v>0.29899999999999999</v>
@@ -7326,7 +7297,7 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B343">
         <v>0.3</v>
@@ -7342,7 +7313,7 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B344">
         <v>0.30099999999999999</v>
@@ -7358,7 +7329,7 @@
     </row>
     <row r="345" spans="1:4">
       <c r="A345" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B345">
         <v>0.30199999999999999</v>
@@ -7374,7 +7345,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="A346" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B346">
         <v>0.30299999999999999</v>
@@ -7390,7 +7361,7 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B347">
         <v>0.36099999999999999</v>
@@ -7406,7 +7377,7 @@
     </row>
     <row r="348" spans="1:4">
       <c r="A348" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B348">
         <v>0.36199999999999999</v>
@@ -7422,7 +7393,7 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B349">
         <v>0.36299999999999999</v>
@@ -7438,7 +7409,7 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B350">
         <v>0.36399999999999999</v>
@@ -7454,7 +7425,7 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B351">
         <v>0.36499999999999999</v>
@@ -7470,7 +7441,7 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B352">
         <v>0.36599999999999999</v>
@@ -7486,7 +7457,7 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B353">
         <v>0.38200000000000001</v>
@@ -7502,7 +7473,7 @@
     </row>
     <row r="354" spans="1:4">
       <c r="A354" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B354">
         <v>0.38300000000000001</v>
@@ -7518,7 +7489,7 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B355">
         <v>0.38400000000000001</v>
@@ -7534,7 +7505,7 @@
     </row>
     <row r="356" spans="1:4">
       <c r="A356" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B356">
         <v>0.38500000000000001</v>
@@ -7550,7 +7521,7 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B357">
         <v>0.38600000000000001</v>
@@ -7566,7 +7537,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B358">
         <v>0.38700000000000001</v>
@@ -7582,7 +7553,7 @@
     </row>
     <row r="359" spans="1:4">
       <c r="A359" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B359">
         <v>0.41399999999999998</v>
@@ -7598,7 +7569,7 @@
     </row>
     <row r="360" spans="1:4">
       <c r="A360" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B360">
         <v>0.41499999999999998</v>
@@ -7614,7 +7585,7 @@
     </row>
     <row r="361" spans="1:4">
       <c r="A361" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B361">
         <v>0.41599999999999998</v>
@@ -7630,7 +7601,7 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B362">
         <v>0.41699999999999998</v>
@@ -7646,7 +7617,7 @@
     </row>
     <row r="363" spans="1:4">
       <c r="A363" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B363">
         <v>0.41799999999999998</v>
@@ -7662,7 +7633,7 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B364">
         <v>0.41899999999999998</v>
@@ -7678,7 +7649,7 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B365">
         <v>0.435</v>
@@ -7694,7 +7665,7 @@
     </row>
     <row r="366" spans="1:4">
       <c r="A366" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B366">
         <v>0.436</v>
@@ -7710,7 +7681,7 @@
     </row>
     <row r="367" spans="1:4">
       <c r="A367" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B367">
         <v>0.437</v>
@@ -7726,7 +7697,7 @@
     </row>
     <row r="368" spans="1:4">
       <c r="A368" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B368">
         <v>0.438</v>
@@ -7742,7 +7713,7 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B369">
         <v>0.439</v>
@@ -7758,7 +7729,7 @@
     </row>
     <row r="370" spans="1:4">
       <c r="A370" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B370">
         <v>0.44</v>
@@ -7774,7 +7745,7 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B371">
         <v>0.45200000000000001</v>
@@ -7790,7 +7761,7 @@
     </row>
     <row r="372" spans="1:4">
       <c r="A372" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B372">
         <v>0.45300000000000001</v>
@@ -7806,7 +7777,7 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B373">
         <v>0.45400000000000001</v>
@@ -7822,7 +7793,7 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B374">
         <v>0.45500000000000002</v>
@@ -7838,7 +7809,7 @@
     </row>
     <row r="375" spans="1:4">
       <c r="A375" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B375">
         <v>0.45600000000000002</v>
@@ -7854,7 +7825,7 @@
     </row>
     <row r="376" spans="1:4">
       <c r="A376" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B376">
         <v>0.45700000000000002</v>
@@ -7870,7 +7841,7 @@
     </row>
     <row r="377" spans="1:4">
       <c r="A377" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B377">
         <v>0.54300000000000004</v>
@@ -7886,7 +7857,7 @@
     </row>
     <row r="378" spans="1:4">
       <c r="A378" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B378">
         <v>0.54400000000000004</v>
@@ -7902,7 +7873,7 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B379">
         <v>0.54500000000000004</v>
@@ -7918,7 +7889,7 @@
     </row>
     <row r="380" spans="1:4">
       <c r="A380" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B380">
         <v>0.54600000000000004</v>
@@ -7934,7 +7905,7 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B381">
         <v>0.54700000000000004</v>
@@ -7950,7 +7921,7 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B382">
         <v>0.54800000000000004</v>
@@ -7966,7 +7937,7 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B383">
         <v>0.88</v>
@@ -7982,7 +7953,7 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B384">
         <v>0.88100000000000001</v>
@@ -7998,7 +7969,7 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B385">
         <v>0.88200000000000001</v>
@@ -8014,7 +7985,7 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B386">
         <v>0.88300000000000001</v>
@@ -8030,7 +8001,7 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B387">
         <v>0.88400000000000001</v>
@@ -8046,7 +8017,7 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B388">
         <v>0.88500000000000001</v>
@@ -8062,7 +8033,7 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B389">
         <v>0.89800000000000002</v>
@@ -8078,7 +8049,7 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B390">
         <v>0.89900000000000002</v>
@@ -8094,7 +8065,7 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B391">
         <v>0.9</v>
@@ -8110,7 +8081,7 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B392">
         <v>0.90100000000000002</v>
@@ -8126,7 +8097,7 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B393">
         <v>0.90200000000000002</v>
@@ -8142,7 +8113,7 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B394">
         <v>0.90300000000000002</v>

</xml_diff>

<commit_message>
Reworked type checking (issue #4). Began integrating data formatting into parsing  (issue #1). Updated test Excel files.
</commit_message>
<xml_diff>
--- a/backend/test/assets/formatting.xlsx
+++ b/backend/test/assets/formatting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23507"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_50FC12B005E796F1B2322BBBB1879748210656A3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_0AD799C407A41998D09C087BBB5AE2007C7B1B90" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="66">
   <si>
     <t>Pattern</t>
   </si>
@@ -101,6 +101,29 @@
   </si>
   <si>
     <t># ?/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Say:"  \"@\, @\" </t>
+  </si>
+  <si>
+    <t>Hello world</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hello </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>world</t>
+    </r>
+  </si>
+  <si>
+    <t>Netflix</t>
   </si>
   <si>
     <t>000.000.000.000</t>
@@ -224,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="51">
+  <numFmts count="52">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.00E+0"/>
@@ -276,8 +299,9 @@
     <numFmt numFmtId="210" formatCode="[mm]"/>
     <numFmt numFmtId="211" formatCode="[sss]"/>
     <numFmt numFmtId="212" formatCode="mm"/>
+    <numFmt numFmtId="213" formatCode="&quot;Say: &quot;\ \&quot;@\,\ @\&quot;\ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -294,6 +318,20 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -322,10 +360,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -391,8 +430,11 @@
     <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -705,17 +747,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -760,7 +802,7 @@
         <v>123.45</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D29" si="1">TEXT(B3, A3)</f>
+        <f t="shared" ref="D3:D28" si="1">TEXT(B3, A3)</f>
         <v>123.45</v>
       </c>
     </row>
@@ -916,7 +958,7 @@
         <v>12345.67</v>
       </c>
       <c r="C13" s="47">
-        <f t="shared" ref="C13:C24" si="2">B13</f>
+        <f t="shared" ref="C13:C28" si="2">B13</f>
         <v>12345.67</v>
       </c>
       <c r="D13" t="str">
@@ -1100,9 +1142,73 @@
         <v xml:space="preserve">1    </v>
       </c>
     </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="65" t="str">
+        <f t="shared" si="2"/>
+        <v>Hello world</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Say:  "Hello world, Hello world" </v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="65" t="str">
+        <f t="shared" si="2"/>
+        <v>Hello world</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Say:  "Hello world, Hello world" </v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="65" t="str">
+        <f t="shared" si="2"/>
+        <v>Netflix</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Say:  "Netflix, Netflix" </v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{E0265B3A-3295-4EF8-8587-112FC168B356}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1142,7 +1248,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1234567890.1229999</v>
@@ -1158,7 +1264,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1234567</v>
@@ -1174,7 +1280,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>123456</v>
@@ -1190,7 +1296,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>123456789</v>
@@ -1206,7 +1312,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>123456789</v>
@@ -1222,7 +1328,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>123456789</v>
@@ -1279,7 +1385,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B2" s="7">
         <v>40867</v>
@@ -1295,7 +1401,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7">
         <v>40868</v>
@@ -1305,13 +1411,13 @@
         <v>40868</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D35" si="1">TEXT(B3, A3)</f>
+        <f t="shared" ref="D3:D34" si="1">TEXT(B3, A3)</f>
         <v>Monday, November 21, 2011</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B4" s="7">
         <v>40869</v>
@@ -1327,7 +1433,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" s="7">
         <v>40870</v>
@@ -1343,7 +1449,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B6" s="7">
         <v>40871</v>
@@ -1359,7 +1465,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B7" s="7">
         <v>40872</v>
@@ -1375,7 +1481,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" s="7">
         <v>40873</v>
@@ -1391,7 +1497,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B9" s="7">
         <v>40874</v>
@@ -1407,7 +1513,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7">
         <v>40875</v>
@@ -1423,7 +1529,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7">
         <v>40876</v>
@@ -1439,7 +1545,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B12" s="7">
         <v>40877</v>
@@ -1455,7 +1561,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B13" s="7">
         <v>40878</v>
@@ -1471,7 +1577,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B14" s="7">
         <v>40879</v>
@@ -1487,7 +1593,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7">
         <v>40880.271701388898</v>
@@ -1503,7 +1609,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B16" s="7">
         <v>40881.271701388891</v>
@@ -1519,7 +1625,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B17" s="7">
         <v>40882.271701388891</v>
@@ -1535,7 +1641,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B18" s="7">
         <v>40883.271701388891</v>
@@ -1551,7 +1657,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B19" s="7">
         <v>40884.271701388891</v>
@@ -1567,7 +1673,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B20" s="7">
         <v>40885.271701388891</v>
@@ -1583,7 +1689,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B21" s="7">
         <v>40886.271701388891</v>
@@ -1599,7 +1705,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B22" s="7">
         <v>40887.271701388891</v>
@@ -1615,7 +1721,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B23" s="7">
         <v>40888.271701388891</v>
@@ -1631,7 +1737,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B24" s="7">
         <v>40889.271707175925</v>
@@ -1647,7 +1753,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B25" s="7">
         <v>40890.271701388891</v>
@@ -1663,7 +1769,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B26" s="7">
         <v>40891.271701388891</v>
@@ -1679,7 +1785,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B27" s="7">
         <v>40892.271701388891</v>
@@ -1695,7 +1801,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B28" s="7">
         <v>40893.271701388891</v>
@@ -1711,7 +1817,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B29" s="7">
         <v>40894.271701388891</v>
@@ -1727,7 +1833,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B30" s="7">
         <v>40895.271701388891</v>
@@ -1743,7 +1849,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B31" s="7">
         <v>25569</v>
@@ -1759,7 +1865,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B32" s="7">
         <v>25569</v>
@@ -1775,7 +1881,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B33" s="7">
         <v>25569</v>
@@ -1791,7 +1897,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B34" s="7">
         <v>40895.271701388891</v>
@@ -1841,7 +1947,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -1857,7 +1963,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>2E-3</v>
@@ -1873,7 +1979,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>3.0000000000000001E-3</v>
@@ -1889,7 +1995,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>4.0000000000000001E-3</v>
@@ -1905,7 +2011,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>5.0000000000000001E-3</v>
@@ -1921,7 +2027,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>6.0000000000000001E-3</v>
@@ -1937,7 +2043,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>7.0000000000000001E-3</v>
@@ -1953,7 +2059,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B9">
         <v>8.0000000000000002E-3</v>
@@ -1969,7 +2075,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <v>8.9999999999999993E-3</v>
@@ -1985,7 +2091,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>0.01</v>
@@ -2001,7 +2107,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B12">
         <v>1.0999999999999999E-2</v>
@@ -2017,7 +2123,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B13">
         <v>1.2E-2</v>
@@ -2033,7 +2139,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>1.2999999999999999E-2</v>
@@ -2049,7 +2155,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>1.4E-2</v>
@@ -2065,7 +2171,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>1.4999999999999999E-2</v>
@@ -2081,7 +2187,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B17">
         <v>1.6E-2</v>
@@ -2097,7 +2203,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18">
         <v>1.7000000000000001E-2</v>
@@ -2113,7 +2219,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>1.7999999999999999E-2</v>
@@ -2129,7 +2235,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>1.9E-2</v>
@@ -2145,7 +2251,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B21">
         <v>0.02</v>
@@ -2161,7 +2267,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B22">
         <v>2.1000000000000001E-2</v>
@@ -2177,7 +2283,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>2.1999999999999999E-2</v>
@@ -2193,7 +2299,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B24">
         <v>2.3E-2</v>
@@ -2209,7 +2315,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B25">
         <v>2.4E-2</v>
@@ -2225,7 +2331,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B26">
         <v>2.5000000000000001E-2</v>
@@ -2241,7 +2347,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>2.5999999999999999E-2</v>
@@ -2257,7 +2363,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B28">
         <v>2.7E-2</v>
@@ -2273,7 +2379,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>2.8000000000000001E-2</v>
@@ -2289,7 +2395,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>2.9000000000000001E-2</v>
@@ -2305,7 +2411,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>0.03</v>
@@ -2321,7 +2427,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>3.1E-2</v>
@@ -2337,7 +2443,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B33">
         <v>3.2000000000000001E-2</v>
@@ -2353,7 +2459,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B34">
         <v>3.3000000000000002E-2</v>
@@ -2369,7 +2475,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>3.4000000000000002E-2</v>
@@ -2385,7 +2491,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B36">
         <v>3.5000000000000003E-2</v>
@@ -2401,7 +2507,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B37">
         <v>3.5999999999999997E-2</v>
@@ -2417,7 +2523,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B38">
         <v>3.6999999999999998E-2</v>
@@ -2433,7 +2539,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>3.7999999999999999E-2</v>
@@ -2449,7 +2555,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B40">
         <v>3.9E-2</v>
@@ -2465,7 +2571,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B41">
         <v>0.04</v>
@@ -2481,7 +2587,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B42">
         <v>4.1000000000000002E-2</v>
@@ -2497,7 +2603,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>4.2000000000000003E-2</v>
@@ -2513,7 +2619,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B44">
         <v>4.2999999999999997E-2</v>
@@ -2529,7 +2635,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B45">
         <v>4.3999999999999997E-2</v>
@@ -2545,7 +2651,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B46">
         <v>4.4999999999999998E-2</v>
@@ -2561,7 +2667,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B47">
         <v>4.5999999999999999E-2</v>
@@ -2577,7 +2683,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B48">
         <v>4.7E-2</v>
@@ -2593,7 +2699,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B49">
         <v>4.8000000000000001E-2</v>
@@ -2609,7 +2715,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B50">
         <v>4.9000000000000002E-2</v>
@@ -2625,7 +2731,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B51">
         <v>0.05</v>
@@ -2641,7 +2747,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B52">
         <v>5.0999999999999997E-2</v>
@@ -2657,7 +2763,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B53">
         <v>5.1999999999999998E-2</v>
@@ -2673,7 +2779,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B54">
         <v>5.2999999999999999E-2</v>
@@ -2689,7 +2795,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B55">
         <v>5.3999999999999999E-2</v>
@@ -2705,7 +2811,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B56">
         <v>5.5E-2</v>
@@ -2721,7 +2827,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B57">
         <v>5.6000000000000001E-2</v>
@@ -2737,7 +2843,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>5.7000000000000002E-2</v>
@@ -2753,7 +2859,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>5.8000000000000003E-2</v>
@@ -2769,7 +2875,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>5.8999999999999997E-2</v>
@@ -2785,7 +2891,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>0.06</v>
@@ -2801,7 +2907,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>6.0999999999999999E-2</v>
@@ -2817,7 +2923,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>6.2E-2</v>
@@ -2833,7 +2939,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>6.3E-2</v>
@@ -2849,7 +2955,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>6.4000000000000001E-2</v>
@@ -2865,7 +2971,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>6.5000000000000002E-2</v>
@@ -2881,7 +2987,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B67">
         <v>6.6000000000000003E-2</v>
@@ -2897,7 +3003,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>6.7000000000000004E-2</v>
@@ -2913,7 +3019,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B69">
         <v>6.8000000000000005E-2</v>
@@ -2929,7 +3035,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B70">
         <v>6.9000000000000006E-2</v>
@@ -2945,7 +3051,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>7.0000000000000007E-2</v>
@@ -2961,7 +3067,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B72">
         <v>7.0999999999999994E-2</v>
@@ -2977,7 +3083,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B73">
         <v>7.1999999999999995E-2</v>
@@ -2993,7 +3099,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B74">
         <v>7.2999999999999995E-2</v>
@@ -3009,7 +3115,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B75">
         <v>7.3999999999999996E-2</v>
@@ -3025,7 +3131,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B76">
         <v>7.4999999999999997E-2</v>
@@ -3041,7 +3147,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B77">
         <v>7.5999999999999998E-2</v>
@@ -3057,7 +3163,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B78">
         <v>7.6999999999999999E-2</v>
@@ -3073,7 +3179,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B79">
         <v>7.8E-2</v>
@@ -3089,7 +3195,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B80">
         <v>7.9000000000000001E-2</v>
@@ -3105,7 +3211,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B81">
         <v>0.08</v>
@@ -3121,7 +3227,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B82">
         <v>8.1000000000000003E-2</v>
@@ -3137,7 +3243,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B83">
         <v>8.2000000000000003E-2</v>
@@ -3153,7 +3259,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B84">
         <v>8.3000000000000004E-2</v>
@@ -3169,7 +3275,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B85">
         <v>8.4000000000000005E-2</v>
@@ -3185,7 +3291,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B86">
         <v>8.5000000000000006E-2</v>
@@ -3201,7 +3307,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B87">
         <v>8.5999999999999993E-2</v>
@@ -3217,7 +3323,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B88">
         <v>8.6999999999999994E-2</v>
@@ -3233,7 +3339,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B89">
         <v>8.7999999999999995E-2</v>
@@ -3249,7 +3355,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B90">
         <v>8.8999999999999996E-2</v>
@@ -3265,7 +3371,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B91">
         <v>0.09</v>
@@ -3281,7 +3387,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B92">
         <v>9.0999999999999998E-2</v>
@@ -3297,7 +3403,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B93">
         <v>9.1999999999999998E-2</v>
@@ -3313,7 +3419,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B94">
         <v>9.2999999999999999E-2</v>
@@ -3329,7 +3435,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B95">
         <v>9.4E-2</v>
@@ -3345,7 +3451,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B96">
         <v>9.5000000000000001E-2</v>
@@ -3361,7 +3467,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B97">
         <v>9.6000000000000002E-2</v>
@@ -3377,7 +3483,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B98">
         <v>9.7000000000000003E-2</v>
@@ -3393,7 +3499,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B99">
         <v>9.8000000000000004E-2</v>
@@ -3409,7 +3515,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B100">
         <v>9.9000000000000005E-2</v>
@@ -3425,7 +3531,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B101">
         <v>0.62</v>
@@ -3441,7 +3547,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B102">
         <v>0.621</v>
@@ -3457,7 +3563,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B103">
         <v>0.622</v>
@@ -3473,7 +3579,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B104">
         <v>0.623</v>
@@ -3489,7 +3595,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B105">
         <v>0.624</v>
@@ -3505,7 +3611,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B106">
         <v>0.625</v>
@@ -3521,7 +3627,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B107">
         <v>0.626</v>
@@ -3537,7 +3643,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B108">
         <v>0.627</v>
@@ -3553,7 +3659,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B109">
         <v>0.628</v>
@@ -3569,7 +3675,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B110">
         <v>0.629</v>
@@ -3585,7 +3691,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B111">
         <v>0.63</v>
@@ -3601,7 +3707,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B112">
         <v>0.63100000000000001</v>
@@ -3617,7 +3723,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B113">
         <v>0.63200000000000001</v>
@@ -3633,7 +3739,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B114">
         <v>0.63300000000000001</v>
@@ -3649,7 +3755,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B115">
         <v>0.63400000000000001</v>
@@ -3665,7 +3771,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B116">
         <v>0.63500000000000001</v>
@@ -3681,7 +3787,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B117">
         <v>0.63600000000000001</v>
@@ -3697,7 +3803,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B118">
         <v>0.63700000000000001</v>
@@ -3713,7 +3819,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B119">
         <v>0.63800000000000001</v>
@@ -3729,7 +3835,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B120">
         <v>0.63900000000000001</v>
@@ -3745,7 +3851,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B121">
         <v>0.64</v>
@@ -3761,7 +3867,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B122">
         <v>0.64100000000000001</v>
@@ -3777,7 +3883,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B123">
         <v>0.64200000000000002</v>
@@ -3793,7 +3899,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B124">
         <v>0.64300000000000002</v>
@@ -3809,7 +3915,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B125">
         <v>0.64400000000000002</v>
@@ -3825,7 +3931,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B126">
         <v>0.64500000000000002</v>
@@ -3841,7 +3947,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B127">
         <v>0.64600000000000002</v>
@@ -3857,7 +3963,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B128">
         <v>0.64700000000000002</v>
@@ -3873,7 +3979,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B129">
         <v>0.64800000000000002</v>
@@ -3889,7 +3995,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B130">
         <v>0.64900000000000002</v>
@@ -3905,7 +4011,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B131">
         <v>0.65</v>
@@ -3921,7 +4027,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B132">
         <v>0.65100000000000002</v>
@@ -3937,7 +4043,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B133">
         <v>0.65200000000000002</v>
@@ -3953,7 +4059,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B134">
         <v>0.65300000000000002</v>
@@ -3969,7 +4075,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B135">
         <v>0.65400000000000003</v>
@@ -3985,7 +4091,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B136">
         <v>0.65500000000000003</v>
@@ -4001,7 +4107,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B137">
         <v>0.65600000000000003</v>
@@ -4017,7 +4123,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B138">
         <v>0.65700000000000003</v>
@@ -4033,7 +4139,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B139">
         <v>0.65800000000000003</v>
@@ -4049,7 +4155,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B140">
         <v>0.65900000000000003</v>
@@ -4065,7 +4171,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B141">
         <v>0.66</v>
@@ -4081,7 +4187,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B142">
         <v>0.66100000000000003</v>
@@ -4097,7 +4203,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B143">
         <v>0.66200000000000003</v>
@@ -4113,7 +4219,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B144">
         <v>0.66300000000000003</v>
@@ -4129,7 +4235,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B145">
         <v>0.66400000000000003</v>
@@ -4145,7 +4251,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B146">
         <v>0.66500000000000004</v>
@@ -4161,7 +4267,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B147">
         <v>0.66600000000000004</v>
@@ -4177,7 +4283,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B148">
         <v>0.66700000000000004</v>
@@ -4193,7 +4299,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B149">
         <v>0.66800000000000004</v>
@@ -4209,7 +4315,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B150">
         <v>0.66900000000000004</v>
@@ -4225,7 +4331,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B151">
         <v>0.67</v>
@@ -4241,7 +4347,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B152">
         <v>0.67100000000000004</v>
@@ -4257,7 +4363,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B153">
         <v>0.67200000000000004</v>
@@ -4273,7 +4379,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B154">
         <v>0.67300000000000004</v>
@@ -4289,7 +4395,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B155">
         <v>0.67400000000000004</v>
@@ -4305,7 +4411,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B156">
         <v>0.67500000000000004</v>
@@ -4321,7 +4427,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B157">
         <v>0.67600000000000005</v>
@@ -4337,7 +4443,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B158">
         <v>0.67700000000000005</v>
@@ -4353,7 +4459,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B159">
         <v>0.67800000000000005</v>
@@ -4369,7 +4475,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B160">
         <v>0.67900000000000005</v>
@@ -4385,7 +4491,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B161">
         <v>0.68</v>
@@ -4401,7 +4507,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B162">
         <v>0.68100000000000005</v>
@@ -4417,7 +4523,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B163">
         <v>0.68200000000000005</v>
@@ -4433,7 +4539,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B164">
         <v>0.68300000000000005</v>
@@ -4449,7 +4555,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B165">
         <v>0.68400000000000005</v>
@@ -4465,7 +4571,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B166">
         <v>0.68500000000000005</v>
@@ -4481,7 +4587,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B167">
         <v>0.68600000000000005</v>
@@ -4497,7 +4603,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B168">
         <v>0.68700000000000006</v>
@@ -4513,7 +4619,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B169">
         <v>0.68799999999999994</v>
@@ -4529,7 +4635,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B170">
         <v>0.68899999999999995</v>
@@ -4545,7 +4651,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B171">
         <v>0.69</v>
@@ -4561,7 +4667,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B172">
         <v>0.69099999999999995</v>
@@ -4577,7 +4683,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B173">
         <v>0.69199999999999995</v>
@@ -4593,7 +4699,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B174">
         <v>0.69299999999999995</v>
@@ -4609,7 +4715,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B175">
         <v>0.69399999999999995</v>
@@ -4625,7 +4731,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B176">
         <v>0.69499999999999995</v>
@@ -4641,7 +4747,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B177">
         <v>0.69599999999999995</v>
@@ -4657,7 +4763,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B178">
         <v>0.69699999999999995</v>
@@ -4673,7 +4779,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B179">
         <v>0.69799999999999995</v>
@@ -4689,7 +4795,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B180">
         <v>0.69899999999999995</v>
@@ -4705,7 +4811,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B181">
         <v>0.7</v>
@@ -4721,7 +4827,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B182">
         <v>0.70099999999999996</v>
@@ -4737,7 +4843,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B183">
         <v>0.70199999999999996</v>
@@ -4753,7 +4859,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B184">
         <v>0.70299999999999996</v>
@@ -4769,7 +4875,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B185">
         <v>0.70399999999999996</v>
@@ -4785,7 +4891,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B186">
         <v>0.70499999999999996</v>
@@ -4801,7 +4907,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B187">
         <v>0.70599999999999996</v>
@@ -4817,7 +4923,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B188">
         <v>0.70699999999999996</v>
@@ -4833,7 +4939,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B189">
         <v>0.70799999999999996</v>
@@ -4849,7 +4955,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B190">
         <v>0.70899999999999996</v>
@@ -4865,7 +4971,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B191">
         <v>0.71</v>
@@ -4881,7 +4987,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B192">
         <v>0.71099999999999997</v>
@@ -4897,7 +5003,7 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B193">
         <v>0.71199999999999997</v>
@@ -4913,7 +5019,7 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B194">
         <v>0.71299999999999997</v>
@@ -4929,7 +5035,7 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B195">
         <v>0.71399999999999997</v>
@@ -4945,7 +5051,7 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B196">
         <v>0.71499999999999997</v>
@@ -4961,7 +5067,7 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B197">
         <v>0.71599999999999997</v>
@@ -4977,7 +5083,7 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B198">
         <v>0.71699999999999997</v>
@@ -4993,7 +5099,7 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B199">
         <v>0.71799999999999997</v>
@@ -5009,7 +5115,7 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B200">
         <v>0.71899999999999997</v>
@@ -5025,7 +5131,7 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B201">
         <v>0.99</v>
@@ -5041,7 +5147,7 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B202">
         <v>0.99099999999999999</v>
@@ -5057,7 +5163,7 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B203">
         <v>0.99199999999999999</v>
@@ -5073,7 +5179,7 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B204">
         <v>0.99299999999999999</v>
@@ -5089,7 +5195,7 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B205">
         <v>0.99399999999999999</v>
@@ -5105,7 +5211,7 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B206">
         <v>0.995</v>
@@ -5121,7 +5227,7 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B207">
         <v>0.996</v>
@@ -5137,7 +5243,7 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B208">
         <v>0.997</v>
@@ -5153,7 +5259,7 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B209">
         <v>0.998</v>
@@ -5169,7 +5275,7 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B210">
         <v>0.999</v>
@@ -5185,7 +5291,7 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -5201,7 +5307,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B212">
         <v>9.5000000000000001E-2</v>
@@ -5217,7 +5323,7 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B213">
         <v>9.6000000000000002E-2</v>
@@ -5233,7 +5339,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B214">
         <v>9.7000000000000003E-2</v>
@@ -5249,7 +5355,7 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B215">
         <v>9.8000000000000004E-2</v>
@@ -5265,7 +5371,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B216">
         <v>9.9000000000000005E-2</v>
@@ -5281,7 +5387,7 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B217">
         <v>0.1</v>
@@ -5297,7 +5403,7 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B218">
         <v>0.10100000000000001</v>
@@ -5313,7 +5419,7 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B219">
         <v>0.10199999999999999</v>
@@ -5329,7 +5435,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B220">
         <v>0.10299999999999999</v>
@@ -5345,7 +5451,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B221">
         <v>0.104</v>
@@ -5361,7 +5467,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B222">
         <v>0.105</v>
@@ -5377,7 +5483,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B223">
         <v>0.106</v>
@@ -5393,7 +5499,7 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B224">
         <v>0.107</v>
@@ -5409,7 +5515,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B225">
         <v>0.108</v>
@@ -5425,7 +5531,7 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B226">
         <v>0.109</v>
@@ -5441,7 +5547,7 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B227">
         <v>0.11</v>
@@ -5457,7 +5563,7 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B228">
         <v>0.111</v>
@@ -5473,7 +5579,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B229">
         <v>0.112</v>
@@ -5489,7 +5595,7 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B230">
         <v>0.113</v>
@@ -5505,7 +5611,7 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B231">
         <v>0.114</v>
@@ -5521,7 +5627,7 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B232">
         <v>0.115</v>
@@ -5537,7 +5643,7 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B233">
         <v>0.11600000000000001</v>
@@ -5553,7 +5659,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B234">
         <v>0.11700000000000001</v>
@@ -5569,7 +5675,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B235">
         <v>0.11799999999999999</v>
@@ -5585,7 +5691,7 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B236">
         <v>0.11899999999999999</v>
@@ -5601,7 +5707,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B237">
         <v>0.12</v>
@@ -5617,7 +5723,7 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B238">
         <v>0.121</v>
@@ -5633,7 +5739,7 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B239">
         <v>0.122</v>
@@ -5649,7 +5755,7 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B240">
         <v>0.123</v>
@@ -5665,7 +5771,7 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B241">
         <v>0.124</v>
@@ -5681,7 +5787,7 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B242">
         <v>0.49</v>
@@ -5697,7 +5803,7 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B243">
         <v>0.49099999999999999</v>
@@ -5713,7 +5819,7 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B244">
         <v>0.49199999999999999</v>
@@ -5729,7 +5835,7 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B245">
         <v>0.49299999999999999</v>
@@ -5745,7 +5851,7 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B246">
         <v>0.49399999999999999</v>
@@ -5761,7 +5867,7 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B247">
         <v>0.495</v>
@@ -5777,7 +5883,7 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B248">
         <v>0.496</v>
@@ -5793,7 +5899,7 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B249">
         <v>0.497</v>
@@ -5809,7 +5915,7 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B250">
         <v>0.498</v>
@@ -5825,7 +5931,7 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B251">
         <v>0.499</v>
@@ -5841,7 +5947,7 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B252">
         <v>0.5</v>
@@ -5857,7 +5963,7 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B253">
         <v>0.501</v>
@@ -5873,7 +5979,7 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B254">
         <v>0.502</v>
@@ -5889,7 +5995,7 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B255">
         <v>0.503</v>
@@ -5905,7 +6011,7 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B256">
         <v>0.504</v>
@@ -5921,7 +6027,7 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B257">
         <v>0.505</v>
@@ -5937,7 +6043,7 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B258">
         <v>0.50600000000000001</v>
@@ -5953,7 +6059,7 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B259">
         <v>0.50700000000000001</v>
@@ -5969,7 +6075,7 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B260">
         <v>0.50800000000000001</v>
@@ -5985,7 +6091,7 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B261">
         <v>0.50900000000000001</v>
@@ -6001,7 +6107,7 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B262">
         <v>0.51</v>
@@ -6017,7 +6123,7 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B263">
         <v>0.51100000000000001</v>
@@ -6033,7 +6139,7 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B264">
         <v>0.51200000000000001</v>
@@ -6049,7 +6155,7 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B265">
         <v>0.51300000000000001</v>
@@ -6065,7 +6171,7 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B266">
         <v>0.51400000000000001</v>
@@ -6081,7 +6187,7 @@
     </row>
     <row r="267" spans="1:4">
       <c r="A267" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B267">
         <v>0.51500000000000001</v>
@@ -6097,7 +6203,7 @@
     </row>
     <row r="268" spans="1:4">
       <c r="A268" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B268">
         <v>0.51600000000000001</v>
@@ -6113,7 +6219,7 @@
     </row>
     <row r="269" spans="1:4">
       <c r="A269" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B269">
         <v>0.51700000000000002</v>
@@ -6129,7 +6235,7 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B270">
         <v>0.51800000000000002</v>
@@ -6145,7 +6251,7 @@
     </row>
     <row r="271" spans="1:4">
       <c r="A271" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B271">
         <v>0.51900000000000002</v>
@@ -6161,7 +6267,7 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B272">
         <v>0.52</v>
@@ -6177,7 +6283,7 @@
     </row>
     <row r="273" spans="1:4">
       <c r="A273" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B273">
         <v>0.97499999999999998</v>
@@ -6193,7 +6299,7 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B274">
         <v>0.97599999999999998</v>
@@ -6209,7 +6315,7 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B275">
         <v>0.97699999999999998</v>
@@ -6225,7 +6331,7 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B276">
         <v>0.97799999999999998</v>
@@ -6241,7 +6347,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B277">
         <v>0.97899999999999998</v>
@@ -6257,7 +6363,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B278">
         <v>0.98</v>
@@ -6273,7 +6379,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B279">
         <v>0.98099999999999998</v>
@@ -6289,7 +6395,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B280">
         <v>0.98199999999999998</v>
@@ -6305,7 +6411,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B281">
         <v>0.98299999999999998</v>
@@ -6321,7 +6427,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B282">
         <v>0.98399999999999999</v>
@@ -6337,7 +6443,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B283">
         <v>0.98499999999999999</v>
@@ -6353,7 +6459,7 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B284">
         <v>0.98599999999999999</v>
@@ -6369,7 +6475,7 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B285">
         <v>0.98699999999999999</v>
@@ -6385,7 +6491,7 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B286">
         <v>0.98799999999999999</v>
@@ -6401,7 +6507,7 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B287">
         <v>0.98899999999999999</v>
@@ -6417,7 +6523,7 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B288">
         <v>0.99</v>
@@ -6433,7 +6539,7 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B289">
         <v>0.99099999999999999</v>
@@ -6449,7 +6555,7 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B290">
         <v>0.99199999999999999</v>
@@ -6465,7 +6571,7 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B291">
         <v>0.99299999999999999</v>
@@ -6481,7 +6587,7 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B292">
         <v>0.99399999999999999</v>
@@ -6497,7 +6603,7 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B293">
         <v>9.8000000000000004E-2</v>
@@ -6513,7 +6619,7 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B294">
         <v>9.9000000000000005E-2</v>
@@ -6529,7 +6635,7 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B295">
         <v>0.1</v>
@@ -6545,7 +6651,7 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B296">
         <v>0.10100000000000001</v>
@@ -6561,7 +6667,7 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B297">
         <v>0.10199999999999999</v>
@@ -6577,7 +6683,7 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B298">
         <v>0.10299999999999999</v>
@@ -6593,7 +6699,7 @@
     </row>
     <row r="299" spans="1:4">
       <c r="A299" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B299">
         <v>0.115</v>
@@ -6609,7 +6715,7 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B300">
         <v>0.11600000000000001</v>
@@ -6625,7 +6731,7 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B301">
         <v>0.11700000000000001</v>
@@ -6641,7 +6747,7 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B302">
         <v>0.11799999999999999</v>
@@ -6657,7 +6763,7 @@
     </row>
     <row r="303" spans="1:4">
       <c r="A303" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B303">
         <v>0.11899999999999999</v>
@@ -6673,7 +6779,7 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B304">
         <v>0.12</v>
@@ -6689,7 +6795,7 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B305">
         <v>0.13100000000000001</v>
@@ -6705,7 +6811,7 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B306">
         <v>0.13200000000000001</v>
@@ -6721,7 +6827,7 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B307">
         <v>0.13300000000000001</v>
@@ -6737,7 +6843,7 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B308">
         <v>0.13400000000000001</v>
@@ -6753,7 +6859,7 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B309">
         <v>0.13500000000000001</v>
@@ -6769,7 +6875,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B310">
         <v>0.13600000000000001</v>
@@ -6785,7 +6891,7 @@
     </row>
     <row r="311" spans="1:4">
       <c r="A311" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B311">
         <v>0.151</v>
@@ -6801,7 +6907,7 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B312">
         <v>0.152</v>
@@ -6817,7 +6923,7 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B313">
         <v>0.153</v>
@@ -6833,7 +6939,7 @@
     </row>
     <row r="314" spans="1:4">
       <c r="A314" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B314">
         <v>0.154</v>
@@ -6849,7 +6955,7 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B315">
         <v>0.155</v>
@@ -6865,7 +6971,7 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B316">
         <v>0.156</v>
@@ -6881,7 +6987,7 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B317">
         <v>0.17899999999999999</v>
@@ -6897,7 +7003,7 @@
     </row>
     <row r="318" spans="1:4">
       <c r="A318" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B318">
         <v>0.18</v>
@@ -6913,7 +7019,7 @@
     </row>
     <row r="319" spans="1:4">
       <c r="A319" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B319">
         <v>0.18099999999999999</v>
@@ -6929,7 +7035,7 @@
     </row>
     <row r="320" spans="1:4">
       <c r="A320" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B320">
         <v>0.182</v>
@@ -6945,7 +7051,7 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B321">
         <v>0.183</v>
@@ -6961,7 +7067,7 @@
     </row>
     <row r="322" spans="1:4">
       <c r="A322" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B322">
         <v>0.184</v>
@@ -6977,7 +7083,7 @@
     </row>
     <row r="323" spans="1:4">
       <c r="A323" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B323">
         <v>0.21199999999999999</v>
@@ -6993,7 +7099,7 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B324">
         <v>0.21299999999999999</v>
@@ -7009,7 +7115,7 @@
     </row>
     <row r="325" spans="1:4">
       <c r="A325" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B325">
         <v>0.214</v>
@@ -7025,7 +7131,7 @@
     </row>
     <row r="326" spans="1:4">
       <c r="A326" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B326">
         <v>0.215</v>
@@ -7041,7 +7147,7 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B327">
         <v>0.216</v>
@@ -7057,7 +7163,7 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B328">
         <v>0.217</v>
@@ -7073,7 +7179,7 @@
     </row>
     <row r="329" spans="1:4">
       <c r="A329" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B329">
         <v>0.22800000000000001</v>
@@ -7089,7 +7195,7 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B330">
         <v>0.22900000000000001</v>
@@ -7105,7 +7211,7 @@
     </row>
     <row r="331" spans="1:4">
       <c r="A331" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B331">
         <v>0.23</v>
@@ -7121,7 +7227,7 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B332">
         <v>0.23100000000000001</v>
@@ -7137,7 +7243,7 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B333">
         <v>0.23200000000000001</v>
@@ -7153,7 +7259,7 @@
     </row>
     <row r="334" spans="1:4">
       <c r="A334" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B334">
         <v>0.23300000000000001</v>
@@ -7169,7 +7275,7 @@
     </row>
     <row r="335" spans="1:4">
       <c r="A335" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B335">
         <v>0.27</v>
@@ -7185,7 +7291,7 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B336">
         <v>0.27100000000000002</v>
@@ -7201,7 +7307,7 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B337">
         <v>0.27200000000000002</v>
@@ -7217,7 +7323,7 @@
     </row>
     <row r="338" spans="1:4">
       <c r="A338" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B338">
         <v>0.27300000000000002</v>
@@ -7233,7 +7339,7 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B339">
         <v>0.27400000000000002</v>
@@ -7249,7 +7355,7 @@
     </row>
     <row r="340" spans="1:4">
       <c r="A340" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B340">
         <v>0.27500000000000002</v>
@@ -7265,7 +7371,7 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B341">
         <v>0.29799999999999999</v>
@@ -7281,7 +7387,7 @@
     </row>
     <row r="342" spans="1:4">
       <c r="A342" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B342">
         <v>0.29899999999999999</v>
@@ -7297,7 +7403,7 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B343">
         <v>0.3</v>
@@ -7313,7 +7419,7 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B344">
         <v>0.30099999999999999</v>
@@ -7329,7 +7435,7 @@
     </row>
     <row r="345" spans="1:4">
       <c r="A345" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B345">
         <v>0.30199999999999999</v>
@@ -7345,7 +7451,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="A346" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B346">
         <v>0.30299999999999999</v>
@@ -7361,7 +7467,7 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B347">
         <v>0.36099999999999999</v>
@@ -7377,7 +7483,7 @@
     </row>
     <row r="348" spans="1:4">
       <c r="A348" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B348">
         <v>0.36199999999999999</v>
@@ -7393,7 +7499,7 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B349">
         <v>0.36299999999999999</v>
@@ -7409,7 +7515,7 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B350">
         <v>0.36399999999999999</v>
@@ -7425,7 +7531,7 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B351">
         <v>0.36499999999999999</v>
@@ -7441,7 +7547,7 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B352">
         <v>0.36599999999999999</v>
@@ -7457,7 +7563,7 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B353">
         <v>0.38200000000000001</v>
@@ -7473,7 +7579,7 @@
     </row>
     <row r="354" spans="1:4">
       <c r="A354" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B354">
         <v>0.38300000000000001</v>
@@ -7489,7 +7595,7 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B355">
         <v>0.38400000000000001</v>
@@ -7505,7 +7611,7 @@
     </row>
     <row r="356" spans="1:4">
       <c r="A356" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B356">
         <v>0.38500000000000001</v>
@@ -7521,7 +7627,7 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B357">
         <v>0.38600000000000001</v>
@@ -7537,7 +7643,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B358">
         <v>0.38700000000000001</v>
@@ -7553,7 +7659,7 @@
     </row>
     <row r="359" spans="1:4">
       <c r="A359" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B359">
         <v>0.41399999999999998</v>
@@ -7569,7 +7675,7 @@
     </row>
     <row r="360" spans="1:4">
       <c r="A360" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B360">
         <v>0.41499999999999998</v>
@@ -7585,7 +7691,7 @@
     </row>
     <row r="361" spans="1:4">
       <c r="A361" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B361">
         <v>0.41599999999999998</v>
@@ -7601,7 +7707,7 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B362">
         <v>0.41699999999999998</v>
@@ -7617,7 +7723,7 @@
     </row>
     <row r="363" spans="1:4">
       <c r="A363" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B363">
         <v>0.41799999999999998</v>
@@ -7633,7 +7739,7 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B364">
         <v>0.41899999999999998</v>
@@ -7649,7 +7755,7 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B365">
         <v>0.435</v>
@@ -7665,7 +7771,7 @@
     </row>
     <row r="366" spans="1:4">
       <c r="A366" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B366">
         <v>0.436</v>
@@ -7681,7 +7787,7 @@
     </row>
     <row r="367" spans="1:4">
       <c r="A367" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B367">
         <v>0.437</v>
@@ -7697,7 +7803,7 @@
     </row>
     <row r="368" spans="1:4">
       <c r="A368" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B368">
         <v>0.438</v>
@@ -7713,7 +7819,7 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B369">
         <v>0.439</v>
@@ -7729,7 +7835,7 @@
     </row>
     <row r="370" spans="1:4">
       <c r="A370" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B370">
         <v>0.44</v>
@@ -7745,7 +7851,7 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B371">
         <v>0.45200000000000001</v>
@@ -7761,7 +7867,7 @@
     </row>
     <row r="372" spans="1:4">
       <c r="A372" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B372">
         <v>0.45300000000000001</v>
@@ -7777,7 +7883,7 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B373">
         <v>0.45400000000000001</v>
@@ -7793,7 +7899,7 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B374">
         <v>0.45500000000000002</v>
@@ -7809,7 +7915,7 @@
     </row>
     <row r="375" spans="1:4">
       <c r="A375" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B375">
         <v>0.45600000000000002</v>
@@ -7825,7 +7931,7 @@
     </row>
     <row r="376" spans="1:4">
       <c r="A376" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B376">
         <v>0.45700000000000002</v>
@@ -7841,7 +7947,7 @@
     </row>
     <row r="377" spans="1:4">
       <c r="A377" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B377">
         <v>0.54300000000000004</v>
@@ -7857,7 +7963,7 @@
     </row>
     <row r="378" spans="1:4">
       <c r="A378" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B378">
         <v>0.54400000000000004</v>
@@ -7873,7 +7979,7 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B379">
         <v>0.54500000000000004</v>
@@ -7889,7 +7995,7 @@
     </row>
     <row r="380" spans="1:4">
       <c r="A380" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B380">
         <v>0.54600000000000004</v>
@@ -7905,7 +8011,7 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B381">
         <v>0.54700000000000004</v>
@@ -7921,7 +8027,7 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B382">
         <v>0.54800000000000004</v>
@@ -7937,7 +8043,7 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B383">
         <v>0.88</v>
@@ -7953,7 +8059,7 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B384">
         <v>0.88100000000000001</v>
@@ -7969,7 +8075,7 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B385">
         <v>0.88200000000000001</v>
@@ -7985,7 +8091,7 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B386">
         <v>0.88300000000000001</v>
@@ -8001,7 +8107,7 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B387">
         <v>0.88400000000000001</v>
@@ -8017,7 +8123,7 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B388">
         <v>0.88500000000000001</v>
@@ -8033,7 +8139,7 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B389">
         <v>0.89800000000000002</v>
@@ -8049,7 +8155,7 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B390">
         <v>0.89900000000000002</v>
@@ -8065,7 +8171,7 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B391">
         <v>0.9</v>
@@ -8081,7 +8187,7 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B392">
         <v>0.90100000000000002</v>
@@ -8097,7 +8203,7 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B393">
         <v>0.90200000000000002</v>
@@ -8113,7 +8219,7 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B394">
         <v>0.90300000000000002</v>

</xml_diff>

<commit_message>
Implemented locale-specific date format (issue #9).
</commit_message>
<xml_diff>
--- a/backend/test/assets/formatting.xlsx
+++ b/backend/test/assets/formatting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21180" windowHeight="10980" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>000-000-00-00</t>
   </si>
   <si>
-    <t>mm-dd-yy</t>
-  </si>
-  <si>
     <t>[$-F800]dddd, mmmm dd, yyyy</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t># ?/?</t>
+  </si>
+  <si>
+    <t>m/d/yyyy</t>
   </si>
 </sst>
 </file>
@@ -894,7 +894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -904,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B2" s="10">
         <v>40867</v>
@@ -1567,12 +1567,12 @@
       </c>
       <c r="D2" s="3" t="str">
         <f>TEXT(B2, A2)</f>
-        <v>11-20-11</v>
+        <v>11/20/2011</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="10">
         <v>40868</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="10">
         <v>40869</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="10">
         <v>40870</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10">
         <v>40871</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10">
         <v>40872</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="10">
         <v>40873</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10">
         <v>40874</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="10">
         <v>40875</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="10">
         <v>40876</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="10">
         <v>40877</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="10">
         <v>40878</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="10">
         <v>40879</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="10">
         <v>40880.271701388898</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="10">
         <v>40881.271701388891</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="10">
         <v>40882.271701388891</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="10">
         <v>40883.271701388891</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="10">
         <v>40884.271701388891</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="10">
         <v>40885.271701388891</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="10">
         <v>40886.271701388891</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="10">
         <v>40887.271701388891</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="10">
         <v>40888.271701388891</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="10">
         <v>40889.271707175925</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="10">
         <v>40890.271701388891</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="10">
         <v>40891.271701388891</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="10">
         <v>40892.271701388891</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="10">
         <v>40893.271701388891</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="10">
         <v>40894.271701388891</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="10">
         <v>40895.271701388891</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="10">
         <v>25569</v>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="10">
         <v>25569</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="10">
         <v>25569</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="10">
         <v>40895.271701388891</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3">
         <v>1E-3</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3">
         <v>2E-3</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3">
         <v>3.0000000000000001E-3</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3">
         <v>4.0000000000000001E-3</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3">
         <v>5.0000000000000001E-3</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3">
         <v>6.0000000000000001E-3</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5">
         <v>7.0000000000000001E-3</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3">
         <v>8.0000000000000002E-3</v>
@@ -2249,7 +2249,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3">
         <v>8.9999999999999993E-3</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3">
         <v>0.01</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3">
         <v>1.0999999999999999E-2</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3">
         <v>1.2E-2</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5">
         <v>1.2999999999999999E-2</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3">
         <v>1.4E-2</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="3">
         <v>1.4999999999999999E-2</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="3">
         <v>1.6E-2</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3">
         <v>1.7000000000000001E-2</v>
@@ -2393,7 +2393,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="3">
         <v>1.7999999999999999E-2</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3">
         <v>1.9E-2</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3">
         <v>0.02</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3">
         <v>2.1000000000000001E-2</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3">
         <v>2.1999999999999999E-2</v>
@@ -2473,7 +2473,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3">
         <v>2.3E-2</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3">
         <v>2.4E-2</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3">
         <v>2.5000000000000001E-2</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="3">
         <v>2.5999999999999999E-2</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3">
         <v>2.7E-2</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="3">
         <v>2.8000000000000001E-2</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3">
         <v>2.9000000000000001E-2</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3">
         <v>0.03</v>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5">
         <v>3.1E-2</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3">
         <v>3.2000000000000001E-2</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3">
         <v>3.3000000000000002E-2</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="3">
         <v>3.4000000000000002E-2</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="3">
         <v>3.5000000000000003E-2</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3">
         <v>3.5999999999999997E-2</v>
@@ -2697,7 +2697,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="3">
         <v>3.6999999999999998E-2</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="3">
         <v>3.7999999999999999E-2</v>
@@ -2729,7 +2729,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5">
         <v>3.9E-2</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3">
         <v>0.04</v>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="5">
         <v>4.1000000000000002E-2</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="3">
         <v>4.2000000000000003E-2</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" s="3">
         <v>4.2999999999999997E-2</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3">
         <v>4.3999999999999997E-2</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" s="3">
         <v>4.4999999999999998E-2</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="3">
         <v>4.5999999999999999E-2</v>
@@ -2857,7 +2857,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="5">
         <v>4.7E-2</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3">
         <v>4.8000000000000001E-2</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" s="3">
         <v>4.9000000000000002E-2</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3">
         <v>0.05</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3">
         <v>5.0999999999999997E-2</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" s="3">
         <v>5.1999999999999998E-2</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="3">
         <v>5.2999999999999999E-2</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="3">
         <v>5.3999999999999999E-2</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B56" s="3">
         <v>5.5E-2</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="3">
         <v>5.6000000000000001E-2</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="3">
         <v>5.7000000000000002E-2</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" s="3">
         <v>5.8000000000000003E-2</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" s="3">
         <v>5.8999999999999997E-2</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61" s="3">
         <v>0.06</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="3">
         <v>6.0999999999999999E-2</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3">
         <v>6.2E-2</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="3">
         <v>6.3E-2</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="3">
         <v>6.4000000000000001E-2</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="3">
         <v>6.5000000000000002E-2</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B67" s="3">
         <v>6.6000000000000003E-2</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" s="3">
         <v>6.7000000000000004E-2</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B69" s="3">
         <v>6.8000000000000005E-2</v>
@@ -3209,7 +3209,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="3">
         <v>6.9000000000000006E-2</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71" s="3">
         <v>7.0000000000000007E-2</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="3">
         <v>7.0999999999999994E-2</v>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B73" s="3">
         <v>7.1999999999999995E-2</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B74" s="3">
         <v>7.2999999999999995E-2</v>
@@ -3289,7 +3289,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B75" s="3">
         <v>7.3999999999999996E-2</v>
@@ -3305,7 +3305,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B76" s="3">
         <v>7.4999999999999997E-2</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" s="3">
         <v>7.5999999999999998E-2</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78" s="3">
         <v>7.6999999999999999E-2</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B79" s="3">
         <v>7.8E-2</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80" s="3">
         <v>7.9000000000000001E-2</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B81" s="3">
         <v>0.08</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B82" s="3">
         <v>8.1000000000000003E-2</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B83" s="3">
         <v>8.2000000000000003E-2</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B84" s="3">
         <v>8.3000000000000004E-2</v>
@@ -3449,7 +3449,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B85" s="3">
         <v>8.4000000000000005E-2</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B86" s="3">
         <v>8.5000000000000006E-2</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B87" s="3">
         <v>8.5999999999999993E-2</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B88" s="3">
         <v>8.6999999999999994E-2</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89" s="3">
         <v>8.7999999999999995E-2</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B90" s="3">
         <v>8.8999999999999996E-2</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B91" s="3">
         <v>0.09</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B92" s="3">
         <v>9.0999999999999998E-2</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B93" s="3">
         <v>9.1999999999999998E-2</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B94" s="3">
         <v>9.2999999999999999E-2</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B95" s="3">
         <v>9.4E-2</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B96" s="3">
         <v>9.5000000000000001E-2</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B97" s="3">
         <v>9.6000000000000002E-2</v>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B98" s="5">
         <v>9.7000000000000003E-2</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B99" s="3">
         <v>9.8000000000000004E-2</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B100" s="3">
         <v>9.9000000000000005E-2</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B101" s="3">
         <v>0.62</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B102" s="3">
         <v>0.621</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B103" s="3">
         <v>0.622</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B104" s="5">
         <v>0.623</v>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B105" s="3">
         <v>0.624</v>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B106" s="3">
         <v>0.625</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B107" s="3">
         <v>0.626</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B108" s="5">
         <v>0.627</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B109" s="3">
         <v>0.628</v>
@@ -3849,7 +3849,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B110" s="3">
         <v>0.629</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B111" s="3">
         <v>0.63</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B112" s="3">
         <v>0.63100000000000001</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113" s="3">
         <v>0.63200000000000001</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B114" s="3">
         <v>0.63300000000000001</v>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B115" s="3">
         <v>0.63400000000000001</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B116" s="3">
         <v>0.63500000000000001</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B117" s="3">
         <v>0.63600000000000001</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B118" s="5">
         <v>0.63700000000000001</v>
@@ -3993,7 +3993,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B119" s="3">
         <v>0.63800000000000001</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B120" s="3">
         <v>0.63900000000000001</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B121" s="3">
         <v>0.64</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B122" s="5">
         <v>0.64100000000000001</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B123" s="3">
         <v>0.64200000000000002</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B124" s="3">
         <v>0.64300000000000002</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B125" s="3">
         <v>0.64400000000000002</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B126" s="3">
         <v>0.64500000000000002</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B127" s="3">
         <v>0.64600000000000002</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B128" s="5">
         <v>0.64700000000000002</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B129" s="3">
         <v>0.64800000000000002</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B130" s="5">
         <v>0.64900000000000002</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B131" s="3">
         <v>0.65</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B132" s="5">
         <v>0.65100000000000002</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B133" s="3">
         <v>0.65200000000000002</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B134" s="3">
         <v>0.65300000000000002</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B135" s="3">
         <v>0.65400000000000003</v>
@@ -4265,7 +4265,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B136" s="3">
         <v>0.65500000000000003</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B137" s="3">
         <v>0.65600000000000003</v>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B138" s="3">
         <v>0.65700000000000003</v>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B139" s="3">
         <v>0.65800000000000003</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B140" s="3">
         <v>0.65900000000000003</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B141" s="3">
         <v>0.66</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B142" s="3">
         <v>0.66100000000000003</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B143" s="3">
         <v>0.66200000000000003</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B144" s="3">
         <v>0.66300000000000003</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B145" s="3">
         <v>0.66400000000000003</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B146" s="3">
         <v>0.66500000000000004</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B147" s="3">
         <v>0.66600000000000004</v>
@@ -4457,7 +4457,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B148" s="3">
         <v>0.66700000000000004</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B149" s="3">
         <v>0.66800000000000004</v>
@@ -4489,7 +4489,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B150" s="3">
         <v>0.66900000000000004</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B151" s="3">
         <v>0.67</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B152" s="5">
         <v>0.67100000000000004</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B153" s="3">
         <v>0.67200000000000004</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B154" s="3">
         <v>0.67300000000000004</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B155" s="3">
         <v>0.67400000000000004</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B156" s="3">
         <v>0.67500000000000004</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B157" s="3">
         <v>0.67600000000000005</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B158" s="3">
         <v>0.67700000000000005</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B159" s="3">
         <v>0.67800000000000005</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B160" s="3">
         <v>0.67900000000000005</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B161" s="3">
         <v>0.68</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B162" s="3">
         <v>0.68100000000000005</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B163" s="3">
         <v>0.68200000000000005</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B164" s="3">
         <v>0.68300000000000005</v>
@@ -4729,7 +4729,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B165" s="3">
         <v>0.68400000000000005</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B166" s="3">
         <v>0.68500000000000005</v>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B167" s="3">
         <v>0.68600000000000005</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B168" s="3">
         <v>0.68700000000000006</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B169" s="3">
         <v>0.68799999999999994</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B170" s="3">
         <v>0.68899999999999995</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B171" s="3">
         <v>0.69</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B172" s="3">
         <v>0.69099999999999995</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B173" s="3">
         <v>0.69199999999999995</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B174" s="3">
         <v>0.69299999999999995</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B175" s="3">
         <v>0.69399999999999995</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B176" s="3">
         <v>0.69499999999999995</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B177" s="3">
         <v>0.69599999999999995</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B178" s="3">
         <v>0.69699999999999995</v>
@@ -4953,7 +4953,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B179" s="3">
         <v>0.69799999999999995</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B180" s="3">
         <v>0.69899999999999995</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B181" s="3">
         <v>0.7</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B182" s="3">
         <v>0.70099999999999996</v>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B183" s="3">
         <v>0.70199999999999996</v>
@@ -5033,7 +5033,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B184" s="3">
         <v>0.70299999999999996</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B185" s="3">
         <v>0.70399999999999996</v>
@@ -5065,7 +5065,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B186" s="3">
         <v>0.70499999999999996</v>
@@ -5081,7 +5081,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B187" s="3">
         <v>0.70599999999999996</v>
@@ -5097,7 +5097,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B188" s="5">
         <v>0.70699999999999996</v>
@@ -5113,7 +5113,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B189" s="3">
         <v>0.70799999999999996</v>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B190" s="3">
         <v>0.70899999999999996</v>
@@ -5145,7 +5145,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B191" s="3">
         <v>0.71</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B192" s="5">
         <v>0.71099999999999997</v>
@@ -5177,7 +5177,7 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B193" s="3">
         <v>0.71199999999999997</v>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B194" s="5">
         <v>0.71299999999999997</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B195" s="3">
         <v>0.71399999999999997</v>
@@ -5225,7 +5225,7 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B196" s="3">
         <v>0.71499999999999997</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B197" s="3">
         <v>0.71599999999999997</v>
@@ -5257,7 +5257,7 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B198" s="3">
         <v>0.71699999999999997</v>
@@ -5273,7 +5273,7 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B199" s="3">
         <v>0.71799999999999997</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B200" s="3">
         <v>0.71899999999999997</v>
@@ -5305,7 +5305,7 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B201" s="3">
         <v>0.99</v>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B202" s="3">
         <v>0.99099999999999999</v>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B203" s="3">
         <v>0.99199999999999999</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B204" s="5">
         <v>0.99299999999999999</v>
@@ -5369,7 +5369,7 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B205" s="3">
         <v>0.99399999999999999</v>
@@ -5385,7 +5385,7 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B206" s="3">
         <v>0.995</v>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B207" s="3">
         <v>0.996</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B208" s="3">
         <v>0.997</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B209" s="3">
         <v>0.998</v>
@@ -5449,7 +5449,7 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B210" s="3">
         <v>0.999</v>
@@ -5465,7 +5465,7 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B211" s="3">
         <v>1</v>
@@ -5481,7 +5481,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B212" s="3">
         <v>9.5000000000000001E-2</v>
@@ -5497,7 +5497,7 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B213" s="3">
         <v>9.6000000000000002E-2</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B214" s="3">
         <v>9.7000000000000003E-2</v>
@@ -5529,7 +5529,7 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B215" s="3">
         <v>9.8000000000000004E-2</v>
@@ -5545,7 +5545,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B216" s="3">
         <v>9.9000000000000005E-2</v>
@@ -5561,7 +5561,7 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B217" s="3">
         <v>0.1</v>
@@ -5577,7 +5577,7 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B218" s="3">
         <v>0.10100000000000001</v>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B219" s="3">
         <v>0.10199999999999999</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B220" s="3">
         <v>0.10299999999999999</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B221" s="5">
         <v>0.104</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B222" s="3">
         <v>0.105</v>
@@ -5657,7 +5657,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B223" s="3">
         <v>0.106</v>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B224" s="3">
         <v>0.107</v>
@@ -5689,7 +5689,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B225" s="3">
         <v>0.108</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B226" s="3">
         <v>0.109</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B227" s="3">
         <v>0.11</v>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B228" s="3">
         <v>0.111</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B229" s="3">
         <v>0.112</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B230" s="3">
         <v>0.113</v>
@@ -5785,7 +5785,7 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B231" s="3">
         <v>0.114</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B232" s="3">
         <v>0.115</v>
@@ -5817,7 +5817,7 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B233" s="3">
         <v>0.11600000000000001</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B234" s="3">
         <v>0.11700000000000001</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B235" s="3">
         <v>0.11799999999999999</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B236" s="3">
         <v>0.11899999999999999</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B237" s="3">
         <v>0.12</v>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B238" s="3">
         <v>0.121</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B239" s="3">
         <v>0.122</v>
@@ -5929,7 +5929,7 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B240" s="3">
         <v>0.123</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B241" s="3">
         <v>0.124</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B242" s="3">
         <v>0.49</v>
@@ -5977,7 +5977,7 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B243" s="3">
         <v>0.49099999999999999</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B244" s="3">
         <v>0.49199999999999999</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B245" s="3">
         <v>0.49299999999999999</v>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B246" s="3">
         <v>0.49399999999999999</v>
@@ -6041,7 +6041,7 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B247" s="3">
         <v>0.495</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B248" s="3">
         <v>0.496</v>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B249" s="3">
         <v>0.497</v>
@@ -6089,7 +6089,7 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B250" s="3">
         <v>0.498</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B251" s="3">
         <v>0.499</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B252" s="3">
         <v>0.5</v>
@@ -6137,7 +6137,7 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B253" s="3">
         <v>0.501</v>
@@ -6153,7 +6153,7 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B254" s="3">
         <v>0.502</v>
@@ -6169,7 +6169,7 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B255" s="3">
         <v>0.503</v>
@@ -6185,7 +6185,7 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B256" s="3">
         <v>0.504</v>
@@ -6201,7 +6201,7 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B257" s="3">
         <v>0.505</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B258" s="3">
         <v>0.50600000000000001</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B259" s="3">
         <v>0.50700000000000001</v>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B260" s="3">
         <v>0.50800000000000001</v>
@@ -6265,7 +6265,7 @@
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B261" s="3">
         <v>0.50900000000000001</v>
@@ -6281,7 +6281,7 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B262" s="3">
         <v>0.51</v>
@@ -6297,7 +6297,7 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B263" s="3">
         <v>0.51100000000000001</v>
@@ -6313,7 +6313,7 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B264" s="3">
         <v>0.51200000000000001</v>
@@ -6329,7 +6329,7 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B265" s="3">
         <v>0.51300000000000001</v>
@@ -6345,7 +6345,7 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B266" s="3">
         <v>0.51400000000000001</v>
@@ -6361,7 +6361,7 @@
     </row>
     <row r="267" spans="1:4">
       <c r="A267" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B267" s="3">
         <v>0.51500000000000001</v>
@@ -6377,7 +6377,7 @@
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B268" s="3">
         <v>0.51600000000000001</v>
@@ -6393,7 +6393,7 @@
     </row>
     <row r="269" spans="1:4">
       <c r="A269" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B269" s="3">
         <v>0.51700000000000002</v>
@@ -6409,7 +6409,7 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B270" s="3">
         <v>0.51800000000000002</v>
@@ -6425,7 +6425,7 @@
     </row>
     <row r="271" spans="1:4">
       <c r="A271" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B271" s="3">
         <v>0.51900000000000002</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B272" s="3">
         <v>0.52</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="273" spans="1:4">
       <c r="A273" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B273" s="3">
         <v>0.97499999999999998</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B274" s="5">
         <v>0.97599999999999998</v>
@@ -6489,7 +6489,7 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B275" s="3">
         <v>0.97699999999999998</v>
@@ -6505,7 +6505,7 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B276" s="3">
         <v>0.97799999999999998</v>
@@ -6521,7 +6521,7 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B277" s="3">
         <v>0.97899999999999998</v>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B278" s="3">
         <v>0.98</v>
@@ -6553,7 +6553,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B279" s="3">
         <v>0.98099999999999998</v>
@@ -6569,7 +6569,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B280" s="3">
         <v>0.98199999999999998</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B281" s="3">
         <v>0.98299999999999998</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B282" s="3">
         <v>0.98399999999999999</v>
@@ -6617,7 +6617,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B283" s="3">
         <v>0.98499999999999999</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B284" s="3">
         <v>0.98599999999999999</v>
@@ -6649,7 +6649,7 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B285" s="3">
         <v>0.98699999999999999</v>
@@ -6665,7 +6665,7 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B286" s="3">
         <v>0.98799999999999999</v>
@@ -6681,7 +6681,7 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B287" s="3">
         <v>0.98899999999999999</v>
@@ -6697,7 +6697,7 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B288" s="3">
         <v>0.99</v>
@@ -6713,7 +6713,7 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B289" s="3">
         <v>0.99099999999999999</v>
@@ -6729,7 +6729,7 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B290" s="3">
         <v>0.99199999999999999</v>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B291" s="3">
         <v>0.99299999999999999</v>
@@ -6761,7 +6761,7 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B292" s="3">
         <v>0.99399999999999999</v>
@@ -6777,7 +6777,7 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B293" s="3">
         <v>9.8000000000000004E-2</v>
@@ -6793,7 +6793,7 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B294" s="3">
         <v>9.9000000000000005E-2</v>
@@ -6809,7 +6809,7 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B295" s="3">
         <v>0.1</v>
@@ -6825,7 +6825,7 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B296" s="3">
         <v>0.10100000000000001</v>
@@ -6841,7 +6841,7 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B297" s="3">
         <v>0.10199999999999999</v>
@@ -6857,7 +6857,7 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B298" s="3">
         <v>0.10299999999999999</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B299" s="3">
         <v>0.115</v>
@@ -6889,7 +6889,7 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B300" s="3">
         <v>0.11600000000000001</v>
@@ -6905,7 +6905,7 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B301" s="3">
         <v>0.11700000000000001</v>
@@ -6921,7 +6921,7 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B302" s="3">
         <v>0.11799999999999999</v>
@@ -6937,7 +6937,7 @@
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B303" s="3">
         <v>0.11899999999999999</v>
@@ -6953,7 +6953,7 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B304" s="3">
         <v>0.12</v>
@@ -6969,7 +6969,7 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B305" s="3">
         <v>0.13100000000000001</v>
@@ -6985,7 +6985,7 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B306" s="3">
         <v>0.13200000000000001</v>
@@ -7001,7 +7001,7 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B307" s="3">
         <v>0.13300000000000001</v>
@@ -7017,7 +7017,7 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B308" s="3">
         <v>0.13400000000000001</v>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B309" s="3">
         <v>0.13500000000000001</v>
@@ -7049,7 +7049,7 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B310" s="3">
         <v>0.13600000000000001</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="311" spans="1:4">
       <c r="A311" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B311" s="3">
         <v>0.151</v>
@@ -7081,7 +7081,7 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B312" s="3">
         <v>0.152</v>
@@ -7097,7 +7097,7 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B313" s="3">
         <v>0.153</v>
@@ -7113,7 +7113,7 @@
     </row>
     <row r="314" spans="1:4">
       <c r="A314" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B314" s="3">
         <v>0.154</v>
@@ -7129,7 +7129,7 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B315" s="3">
         <v>0.155</v>
@@ -7145,7 +7145,7 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B316" s="3">
         <v>0.156</v>
@@ -7161,7 +7161,7 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B317" s="3">
         <v>0.17899999999999999</v>
@@ -7177,7 +7177,7 @@
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B318" s="3">
         <v>0.18</v>
@@ -7193,7 +7193,7 @@
     </row>
     <row r="319" spans="1:4">
       <c r="A319" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B319" s="3">
         <v>0.18099999999999999</v>
@@ -7209,7 +7209,7 @@
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B320" s="3">
         <v>0.182</v>
@@ -7225,7 +7225,7 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B321" s="3">
         <v>0.183</v>
@@ -7241,7 +7241,7 @@
     </row>
     <row r="322" spans="1:4">
       <c r="A322" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B322" s="3">
         <v>0.184</v>
@@ -7257,7 +7257,7 @@
     </row>
     <row r="323" spans="1:4">
       <c r="A323" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B323" s="3">
         <v>0.21199999999999999</v>
@@ -7273,7 +7273,7 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B324" s="3">
         <v>0.21299999999999999</v>
@@ -7289,7 +7289,7 @@
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B325" s="3">
         <v>0.214</v>
@@ -7305,7 +7305,7 @@
     </row>
     <row r="326" spans="1:4">
       <c r="A326" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B326" s="3">
         <v>0.215</v>
@@ -7321,7 +7321,7 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B327" s="3">
         <v>0.216</v>
@@ -7337,7 +7337,7 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B328" s="3">
         <v>0.217</v>
@@ -7353,7 +7353,7 @@
     </row>
     <row r="329" spans="1:4">
       <c r="A329" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B329" s="3">
         <v>0.22800000000000001</v>
@@ -7369,7 +7369,7 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B330" s="3">
         <v>0.22900000000000001</v>
@@ -7385,7 +7385,7 @@
     </row>
     <row r="331" spans="1:4">
       <c r="A331" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B331" s="3">
         <v>0.23</v>
@@ -7401,7 +7401,7 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B332" s="3">
         <v>0.23100000000000001</v>
@@ -7417,7 +7417,7 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B333" s="3">
         <v>0.23200000000000001</v>
@@ -7433,7 +7433,7 @@
     </row>
     <row r="334" spans="1:4">
       <c r="A334" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B334" s="3">
         <v>0.23300000000000001</v>
@@ -7449,7 +7449,7 @@
     </row>
     <row r="335" spans="1:4">
       <c r="A335" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B335" s="3">
         <v>0.27</v>
@@ -7465,7 +7465,7 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B336" s="3">
         <v>0.27100000000000002</v>
@@ -7481,7 +7481,7 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B337" s="3">
         <v>0.27200000000000002</v>
@@ -7497,7 +7497,7 @@
     </row>
     <row r="338" spans="1:4">
       <c r="A338" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B338" s="3">
         <v>0.27300000000000002</v>
@@ -7513,7 +7513,7 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B339" s="3">
         <v>0.27400000000000002</v>
@@ -7529,7 +7529,7 @@
     </row>
     <row r="340" spans="1:4">
       <c r="A340" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B340" s="3">
         <v>0.27500000000000002</v>
@@ -7545,7 +7545,7 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B341" s="3">
         <v>0.29799999999999999</v>
@@ -7561,7 +7561,7 @@
     </row>
     <row r="342" spans="1:4">
       <c r="A342" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B342" s="3">
         <v>0.29899999999999999</v>
@@ -7577,7 +7577,7 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B343" s="3">
         <v>0.3</v>
@@ -7593,7 +7593,7 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B344" s="3">
         <v>0.30099999999999999</v>
@@ -7609,7 +7609,7 @@
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B345" s="3">
         <v>0.30199999999999999</v>
@@ -7625,7 +7625,7 @@
     </row>
     <row r="346" spans="1:4">
       <c r="A346" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B346" s="3">
         <v>0.30299999999999999</v>
@@ -7641,7 +7641,7 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B347" s="3">
         <v>0.36099999999999999</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="348" spans="1:4">
       <c r="A348" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B348" s="3">
         <v>0.36199999999999999</v>
@@ -7673,7 +7673,7 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B349" s="3">
         <v>0.36299999999999999</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B350" s="3">
         <v>0.36399999999999999</v>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B351" s="3">
         <v>0.36499999999999999</v>
@@ -7721,7 +7721,7 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B352" s="3">
         <v>0.36599999999999999</v>
@@ -7737,7 +7737,7 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B353" s="3">
         <v>0.38200000000000001</v>
@@ -7753,7 +7753,7 @@
     </row>
     <row r="354" spans="1:4">
       <c r="A354" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B354" s="3">
         <v>0.38300000000000001</v>
@@ -7769,7 +7769,7 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B355" s="3">
         <v>0.38400000000000001</v>
@@ -7785,7 +7785,7 @@
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B356" s="3">
         <v>0.38500000000000001</v>
@@ -7801,7 +7801,7 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B357" s="3">
         <v>0.38600000000000001</v>
@@ -7817,7 +7817,7 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B358" s="3">
         <v>0.38700000000000001</v>
@@ -7833,7 +7833,7 @@
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B359" s="3">
         <v>0.41399999999999998</v>
@@ -7849,7 +7849,7 @@
     </row>
     <row r="360" spans="1:4">
       <c r="A360" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B360" s="3">
         <v>0.41499999999999998</v>
@@ -7865,7 +7865,7 @@
     </row>
     <row r="361" spans="1:4">
       <c r="A361" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B361" s="3">
         <v>0.41599999999999998</v>
@@ -7881,7 +7881,7 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B362" s="3">
         <v>0.41699999999999998</v>
@@ -7897,7 +7897,7 @@
     </row>
     <row r="363" spans="1:4">
       <c r="A363" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B363" s="3">
         <v>0.41799999999999998</v>
@@ -7913,7 +7913,7 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B364" s="3">
         <v>0.41899999999999998</v>
@@ -7929,7 +7929,7 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B365" s="3">
         <v>0.435</v>
@@ -7945,7 +7945,7 @@
     </row>
     <row r="366" spans="1:4">
       <c r="A366" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B366" s="3">
         <v>0.436</v>
@@ -7961,7 +7961,7 @@
     </row>
     <row r="367" spans="1:4">
       <c r="A367" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B367" s="3">
         <v>0.437</v>
@@ -7977,7 +7977,7 @@
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B368" s="3">
         <v>0.438</v>
@@ -7993,7 +7993,7 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B369" s="3">
         <v>0.439</v>
@@ -8009,7 +8009,7 @@
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B370" s="3">
         <v>0.44</v>
@@ -8025,7 +8025,7 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B371" s="3">
         <v>0.45200000000000001</v>
@@ -8041,7 +8041,7 @@
     </row>
     <row r="372" spans="1:4">
       <c r="A372" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B372" s="3">
         <v>0.45300000000000001</v>
@@ -8057,7 +8057,7 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B373" s="3">
         <v>0.45400000000000001</v>
@@ -8073,7 +8073,7 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B374" s="3">
         <v>0.45500000000000002</v>
@@ -8089,7 +8089,7 @@
     </row>
     <row r="375" spans="1:4">
       <c r="A375" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B375" s="3">
         <v>0.45600000000000002</v>
@@ -8105,7 +8105,7 @@
     </row>
     <row r="376" spans="1:4">
       <c r="A376" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B376" s="3">
         <v>0.45700000000000002</v>
@@ -8121,7 +8121,7 @@
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B377" s="3">
         <v>0.54300000000000004</v>
@@ -8137,7 +8137,7 @@
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B378" s="3">
         <v>0.54400000000000004</v>
@@ -8153,7 +8153,7 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B379" s="3">
         <v>0.54500000000000004</v>
@@ -8169,7 +8169,7 @@
     </row>
     <row r="380" spans="1:4">
       <c r="A380" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B380" s="3">
         <v>0.54600000000000004</v>
@@ -8185,7 +8185,7 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B381" s="3">
         <v>0.54700000000000004</v>
@@ -8201,7 +8201,7 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B382" s="3">
         <v>0.54800000000000004</v>
@@ -8217,7 +8217,7 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B383" s="3">
         <v>0.88</v>
@@ -8233,7 +8233,7 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B384" s="3">
         <v>0.88100000000000001</v>
@@ -8249,7 +8249,7 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B385" s="3">
         <v>0.88200000000000001</v>
@@ -8265,7 +8265,7 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B386" s="3">
         <v>0.88300000000000001</v>
@@ -8281,7 +8281,7 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B387" s="3">
         <v>0.88400000000000001</v>
@@ -8297,7 +8297,7 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B388" s="3">
         <v>0.88500000000000001</v>
@@ -8313,7 +8313,7 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B389" s="3">
         <v>0.89800000000000002</v>
@@ -8329,7 +8329,7 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B390" s="3">
         <v>0.89900000000000002</v>
@@ -8345,7 +8345,7 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B391" s="3">
         <v>0.9</v>
@@ -8361,7 +8361,7 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B392" s="3">
         <v>0.90100000000000002</v>
@@ -8377,7 +8377,7 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B393" s="3">
         <v>0.90200000000000002</v>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B394" s="3">
         <v>0.90300000000000002</v>

</xml_diff>